<commit_message>
#8 could import lots of private info by xlsx
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE748587-152E-CB49-B866-A4A2917E5412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64A170E-C57E-C648-AA3C-D9820B2E823C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,11 @@
     <sheet name="userlessontable" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>username</t>
   </si>
@@ -242,13 +241,45 @@
   </si>
   <si>
     <t>examUsedTime</t>
+  </si>
+  <si>
+    <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test@123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理部门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很牛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +305,14 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,18 +347,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -619,102 +666,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AC1"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="7" width="8.83203125" style="4"/>
+    <col min="8" max="8" width="21.83203125" style="4" customWidth="1"/>
+    <col min="9" max="11" width="8.83203125" style="4"/>
+    <col min="12" max="12" width="16" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.83203125" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:29" s="1" customFormat="1">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:28" s="6" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="X2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{BB6D0120-9F40-7341-B167-31CE7F1D15B8}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -819,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#6 add session getting test case
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64A170E-C57E-C648-AA3C-D9820B2E823C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A7D9B-DBFF-5A4B-8457-80A9FCD71F74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="207" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -677,7 +677,7 @@
     <col min="1" max="7" width="8.83203125" style="4"/>
     <col min="8" max="8" width="21.83203125" style="4" customWidth="1"/>
     <col min="9" max="11" width="8.83203125" style="4"/>
-    <col min="12" max="12" width="16" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" style="4" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="4" customWidth="1"/>
     <col min="14" max="17" width="8.83203125" style="4"/>
     <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
just for a unsaved file, otherwise can not check out
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39828D9-4DD2-A347-9DD4-C6B236D88784}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A747A8-C3E1-5646-BCBC-D4964FFCCC66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5128,7 +5128,7 @@
   <dimension ref="B1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
#13 more six tables read in db fuction writed, test success
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A747A8-C3E1-5646-BCBC-D4964FFCCC66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7844B83C-67C8-0F4A-9546-C4DB9CB5D970}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19700" windowHeight="28800" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="220">
   <si>
     <t>username</t>
   </si>
@@ -701,6 +701,80 @@
   </si>
   <si>
     <t>lession2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin3</t>
+  </si>
+  <si>
+    <t>admin4</t>
+  </si>
+  <si>
+    <t>admin5</t>
+  </si>
+  <si>
+    <t>admin6</t>
+  </si>
+  <si>
+    <t>admin7</t>
+  </si>
+  <si>
+    <t>admin8</t>
+  </si>
+  <si>
+    <t>admin9</t>
+  </si>
+  <si>
+    <t>admin10</t>
+  </si>
+  <si>
+    <t>admin11</t>
+  </si>
+  <si>
+    <t>admin12</t>
+  </si>
+  <si>
+    <t>课件1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www.baidu.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>django</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -788,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -801,6 +875,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1106,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB40"/>
   <sheetViews>
-    <sheetView zoomScale="207" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A28"/>
+    <sheetView topLeftCell="S1" zoomScale="207" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3465,7 +3540,7 @@
     </row>
     <row r="29" spans="1:28">
       <c r="A29" s="4" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>130</v>
@@ -3548,10 +3623,10 @@
     </row>
     <row r="30" spans="1:28">
       <c r="A30" s="4" t="s">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>70</v>
@@ -3631,7 +3706,7 @@
     </row>
     <row r="31" spans="1:28">
       <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>201</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>130</v>
@@ -3714,7 +3789,7 @@
     </row>
     <row r="32" spans="1:28">
       <c r="A32" s="4" t="s">
-        <v>70</v>
+        <v>202</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>130</v>
@@ -3797,7 +3872,7 @@
     </row>
     <row r="33" spans="1:28">
       <c r="A33" s="4" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>130</v>
@@ -3880,7 +3955,7 @@
     </row>
     <row r="34" spans="1:28">
       <c r="A34" s="4" t="s">
-        <v>70</v>
+        <v>204</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>130</v>
@@ -3963,7 +4038,7 @@
     </row>
     <row r="35" spans="1:28">
       <c r="A35" s="4" t="s">
-        <v>70</v>
+        <v>205</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>130</v>
@@ -4046,7 +4121,7 @@
     </row>
     <row r="36" spans="1:28">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>206</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>130</v>
@@ -4129,7 +4204,7 @@
     </row>
     <row r="37" spans="1:28">
       <c r="A37" s="4" t="s">
-        <v>70</v>
+        <v>207</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>130</v>
@@ -4212,7 +4287,7 @@
     </row>
     <row r="38" spans="1:28">
       <c r="A38" s="4" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>130</v>
@@ -4295,7 +4370,7 @@
     </row>
     <row r="39" spans="1:28">
       <c r="A39" s="4" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>130</v>
@@ -4378,7 +4453,7 @@
     </row>
     <row r="40" spans="1:28">
       <c r="A40" s="4" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>130</v>
@@ -4510,41 +4585,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="1" customFormat="1">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:10" s="6" customFormat="1">
+      <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -4552,16 +4629,28 @@
       <c r="B2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2">
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="4">
         <v>2</v>
       </c>
     </row>
@@ -4569,16 +4658,25 @@
       <c r="B3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4">
         <v>3</v>
       </c>
     </row>
@@ -4586,16 +4684,25 @@
       <c r="B4" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="4">
         <v>4</v>
       </c>
     </row>
@@ -4603,16 +4710,25 @@
       <c r="B5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="4">
         <v>5</v>
       </c>
     </row>
@@ -4620,16 +4736,25 @@
       <c r="B6" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="4">
         <v>6</v>
       </c>
     </row>
@@ -4637,19 +4762,25 @@
       <c r="B7" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7">
+      <c r="D7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="4">
         <v>7</v>
       </c>
     </row>
@@ -4657,19 +4788,25 @@
       <c r="B8" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8">
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="4">
         <v>8</v>
       </c>
     </row>
@@ -4677,19 +4814,25 @@
       <c r="B9" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>2</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9">
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="4">
         <v>9</v>
       </c>
     </row>
@@ -4697,19 +4840,25 @@
       <c r="B10" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10">
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="4">
         <v>9</v>
       </c>
     </row>
@@ -4717,19 +4866,25 @@
       <c r="B11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11">
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="4">
         <v>1</v>
       </c>
     </row>
@@ -4737,19 +4892,25 @@
       <c r="B12" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12">
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="4">
         <v>2</v>
       </c>
     </row>
@@ -4763,7 +4924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="221" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="221" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -5127,8 +5288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="302" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5214,8 +5375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="295" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="F1" zoomScale="295" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5317,8 +5478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="370" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="D1" zoomScale="262" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5435,44 +5596,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScale="291" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="194" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="1" max="4" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="12" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="4"/>
     <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -5480,28 +5644,28 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>400</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -5509,28 +5673,28 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>4000</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -5547,8 +5711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScale="214" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="M1" zoomScale="214" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5654,6 +5818,9 @@
       <c r="O2" s="4" t="s">
         <v>173</v>
       </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
       <c r="Q2" t="s">
         <v>191</v>
       </c>
@@ -5694,6 +5861,9 @@
       </c>
       <c r="O3" s="4" t="s">
         <v>86</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>192</v>
@@ -5798,7 +5968,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5889,15 +6059,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="304" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="E1" zoomScale="304" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
@@ -5910,67 +6086,108 @@
       <c r="E1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>56</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{BF5212CB-FD3F-A64E-8797-E33F65D03E11}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:C5"/>
+  <dimension ref="B1:D5"/>
   <sheetViews>
     <sheetView zoomScale="250" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:4" s="6" customFormat="1">
+      <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
+      <c r="D1" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#14 newcomer list completed
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04118AB6-7993-324F-8FCB-35A704ECE123}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3138A6E-599D-FE4E-875F-8781074185F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19700" windowHeight="28800" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="249">
   <si>
     <t>username</t>
   </si>
@@ -840,6 +840,34 @@
   </si>
   <si>
     <t>23</t>
+  </si>
+  <si>
+    <t>HRBP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:33</t>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:34</t>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:35</t>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:36</t>
   </si>
 </sst>
 </file>
@@ -1243,18 +1271,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="207" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="6" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="4" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
@@ -4596,6 +4626,290 @@
       </c>
       <c r="AB40" s="4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
+      <c r="A41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="S41" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="U41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA41" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB41" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
+      <c r="A42" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="S42" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="U42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="X42" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="Z42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA42" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB42" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="A43" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="S43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="X43" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA43" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB43" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
+      <c r="A44" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="S44" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4627,19 +4941,23 @@
     <hyperlink ref="B19" r:id="rId24" xr:uid="{EB596304-69F5-3B49-A9CA-EBACC3AC12CC}"/>
     <hyperlink ref="B26" r:id="rId25" xr:uid="{6F06B90D-083E-0340-B497-56D1D4D55ADB}"/>
     <hyperlink ref="B33" r:id="rId26" xr:uid="{157D968C-75D9-C74E-A39E-57030F2494B6}"/>
-    <hyperlink ref="B40" r:id="rId27" xr:uid="{47567539-6DF2-8945-B4B3-46CF3F2A5181}"/>
-    <hyperlink ref="B13" r:id="rId28" xr:uid="{7EF19AA1-0357-3E4C-842F-5346784BB75F}"/>
-    <hyperlink ref="B20" r:id="rId29" xr:uid="{0FAB670C-22FB-7544-934B-40133CE7B5D5}"/>
-    <hyperlink ref="B27" r:id="rId30" xr:uid="{D6A74CDB-E8A4-B048-8F0F-0F66096D7706}"/>
-    <hyperlink ref="B34" r:id="rId31" xr:uid="{E8D26900-FD62-E74F-AF70-925EB5B8D2B6}"/>
-    <hyperlink ref="B14" r:id="rId32" xr:uid="{5B5B9AC6-1A54-8543-B622-BAC7EBBC387A}"/>
-    <hyperlink ref="B21" r:id="rId33" xr:uid="{BD392BE5-E86F-134D-9956-17BD788E6D07}"/>
-    <hyperlink ref="B28" r:id="rId34" xr:uid="{A3D1F11D-1D90-6643-B1DB-28EC5AE033E9}"/>
-    <hyperlink ref="B35" r:id="rId35" xr:uid="{231521A9-8DDB-2648-9C1E-7C1870420DB6}"/>
-    <hyperlink ref="B15" r:id="rId36" xr:uid="{1CE83D9B-28C3-8742-94DD-66814196C0FA}"/>
-    <hyperlink ref="B22" r:id="rId37" xr:uid="{612FBA4C-0E78-CC47-83BC-F6DDE5E5E461}"/>
-    <hyperlink ref="B29" r:id="rId38" xr:uid="{508EDFD8-2CEB-B74F-900C-175B67214779}"/>
-    <hyperlink ref="B36" r:id="rId39" xr:uid="{8FB6E29E-380E-E542-AA5B-8C9B1E9E4E47}"/>
+    <hyperlink ref="B13" r:id="rId27" xr:uid="{7EF19AA1-0357-3E4C-842F-5346784BB75F}"/>
+    <hyperlink ref="B20" r:id="rId28" xr:uid="{0FAB670C-22FB-7544-934B-40133CE7B5D5}"/>
+    <hyperlink ref="B27" r:id="rId29" xr:uid="{D6A74CDB-E8A4-B048-8F0F-0F66096D7706}"/>
+    <hyperlink ref="B34" r:id="rId30" xr:uid="{E8D26900-FD62-E74F-AF70-925EB5B8D2B6}"/>
+    <hyperlink ref="B14" r:id="rId31" xr:uid="{5B5B9AC6-1A54-8543-B622-BAC7EBBC387A}"/>
+    <hyperlink ref="B21" r:id="rId32" xr:uid="{BD392BE5-E86F-134D-9956-17BD788E6D07}"/>
+    <hyperlink ref="B28" r:id="rId33" xr:uid="{A3D1F11D-1D90-6643-B1DB-28EC5AE033E9}"/>
+    <hyperlink ref="B35" r:id="rId34" xr:uid="{231521A9-8DDB-2648-9C1E-7C1870420DB6}"/>
+    <hyperlink ref="B15" r:id="rId35" xr:uid="{1CE83D9B-28C3-8742-94DD-66814196C0FA}"/>
+    <hyperlink ref="B22" r:id="rId36" xr:uid="{612FBA4C-0E78-CC47-83BC-F6DDE5E5E461}"/>
+    <hyperlink ref="B29" r:id="rId37" xr:uid="{508EDFD8-2CEB-B74F-900C-175B67214779}"/>
+    <hyperlink ref="B36" r:id="rId38" xr:uid="{8FB6E29E-380E-E542-AA5B-8C9B1E9E4E47}"/>
+    <hyperlink ref="B41" r:id="rId39" xr:uid="{BA23BE46-3726-8B44-A6B9-C5E8A5782A4B}"/>
+    <hyperlink ref="B42" r:id="rId40" xr:uid="{B0E5CA72-C47A-644F-8BF7-29588ADFD7C5}"/>
+    <hyperlink ref="B43" r:id="rId41" xr:uid="{6BDE2B2B-396F-9646-A14A-A47A4CBDF0FD}"/>
+    <hyperlink ref="B40" r:id="rId42" xr:uid="{9BE6E5DB-9ED5-D445-A82F-149B56DE779C}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{3DA1C4FE-DC71-3647-B52C-E065CA59C3B0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5821,7 +6139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
+    <sheetView zoomScale="302" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#13 fix write db test, add url, more test applicated
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3138A6E-599D-FE4E-875F-8781074185F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED3AF74-3C73-AF4E-839B-570B66AA82DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1273,14 +1273,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="207" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
@@ -1289,7 +1289,7 @@
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
     <col min="14" max="17" width="8.83203125" style="4"/>
     <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
     <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
#18 #14 now teacher lists is work for frontend
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED3AF74-3C73-AF4E-839B-570B66AA82DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9AC97-1285-C744-8673-96FDECE3A7FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="250">
   <si>
     <t>username</t>
   </si>
@@ -868,6 +868,9 @@
   </si>
   <si>
     <t>2020-12-12 00:00:36</t>
+  </si>
+  <si>
+    <t>admin13</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1277,7 @@
   <dimension ref="A1:AB44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3640,7 +3643,7 @@
         <v>129</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>71</v>
@@ -3723,7 +3726,7 @@
         <v>70</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>71</v>
@@ -3806,7 +3809,7 @@
         <v>129</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>71</v>
@@ -3889,7 +3892,7 @@
         <v>129</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>69</v>
+        <v>201</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>71</v>
@@ -3972,7 +3975,7 @@
         <v>129</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>71</v>
@@ -4055,7 +4058,7 @@
         <v>129</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>69</v>
+        <v>203</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>71</v>
@@ -4138,7 +4141,7 @@
         <v>129</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>69</v>
+        <v>204</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>71</v>
@@ -4221,7 +4224,7 @@
         <v>129</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>69</v>
+        <v>205</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>71</v>
@@ -4304,7 +4307,7 @@
         <v>129</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>69</v>
+        <v>206</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>71</v>
@@ -4387,7 +4390,7 @@
         <v>129</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>71</v>
@@ -4470,7 +4473,7 @@
         <v>129</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>69</v>
+        <v>208</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>71</v>
@@ -4553,7 +4556,7 @@
         <v>129</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>69</v>
+        <v>209</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>71</v>
@@ -4636,7 +4639,7 @@
         <v>129</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>69</v>
+        <v>249</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
#18 #23 now work well with accept and reject nomination #14 list work well with frontend
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9AC97-1285-C744-8673-96FDECE3A7FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C874B3-2816-6941-88B0-61ABF5837666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="H29" zoomScale="207" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4660,7 +4660,7 @@
         <v>128</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="P41" s="4" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
#24 add assign_teacher api, tests is done, now connect with frontend
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C874B3-2816-6941-88B0-61ABF5837666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5DF5D3-B9E1-9846-B283-EFD831942D47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="250">
   <si>
     <t>username</t>
   </si>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H29" zoomScale="207" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" topLeftCell="W10" zoomScale="207" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3205,13 +3205,13 @@
         <v>94</v>
       </c>
       <c r="X23" s="4" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="Y23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="Z23" s="4" t="b">
-        <v>1</v>
+      <c r="Z23" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA23" s="4" t="s">
         <v>94</v>
@@ -3288,13 +3288,13 @@
         <v>95</v>
       </c>
       <c r="X24" s="4" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="Y24" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="Z24" s="4" t="b">
-        <v>1</v>
+      <c r="Z24" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA24" s="4" t="s">
         <v>95</v>
@@ -3371,13 +3371,13 @@
         <v>96</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="Y25" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="Z25" s="4" t="b">
-        <v>1</v>
+      <c r="Z25" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA25" s="4" t="s">
         <v>96</v>
@@ -3454,13 +3454,13 @@
         <v>97</v>
       </c>
       <c r="X26" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="Y26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Z26" s="4" t="b">
-        <v>1</v>
+      <c r="Z26" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA26" s="4" t="s">
         <v>97</v>
@@ -3537,13 +3537,13 @@
         <v>98</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="Y27" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z27" s="4" t="b">
-        <v>1</v>
+      <c r="Z27" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA27" s="4" t="s">
         <v>98</v>
@@ -3620,13 +3620,13 @@
         <v>99</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="Y28" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Z28" s="4" t="b">
-        <v>1</v>
+      <c r="Z28" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AA28" s="4" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
#27 finish bootcamp join in dimension
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70977526-5ABF-46EF-BDE1-049A5972EF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D8BB7-D45E-466A-93A7-5631D50DFEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30735" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="260">
   <si>
     <t>username</t>
   </si>
@@ -871,6 +871,44 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>2022-5-1 00:00:00</t>
+  </si>
+  <si>
+    <t>2022-5-1 00:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-1 23:59:59</t>
+  </si>
+  <si>
+    <t>2022-5-1 23:59:59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-2 00:00:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-4 00:00:02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-5 00:00:03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1276,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="207" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1414,7 +1452,7 @@
         <v>71</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>73</v>
+        <v>251</v>
       </c>
       <c r="I2" s="4">
         <v>1</v>
@@ -1497,7 +1535,7 @@
         <v>71</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>73</v>
+        <v>251</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
@@ -1580,7 +1618,7 @@
         <v>71</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
@@ -1663,7 +1701,7 @@
         <v>71</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
@@ -1746,7 +1784,7 @@
         <v>71</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
@@ -1829,7 +1867,7 @@
         <v>71</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>73</v>
+        <v>253</v>
       </c>
       <c r="I7" s="4">
         <v>1</v>
@@ -1912,7 +1950,7 @@
         <v>71</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>73</v>
+        <v>253</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -1995,7 +2033,7 @@
         <v>71</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>78</v>
+        <v>252</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>126</v>
@@ -2078,7 +2116,7 @@
         <v>71</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>79</v>
+        <v>254</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>126</v>
@@ -2161,7 +2199,7 @@
         <v>71</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>80</v>
+        <v>255</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>126</v>
@@ -2244,7 +2282,7 @@
         <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>81</v>
+        <v>256</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>126</v>
@@ -2327,7 +2365,7 @@
         <v>71</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>82</v>
+        <v>257</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>126</v>
@@ -2410,7 +2448,7 @@
         <v>71</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>83</v>
+        <v>258</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>126</v>
@@ -2493,7 +2531,7 @@
         <v>71</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>126</v>
@@ -2576,7 +2614,7 @@
         <v>71</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>126</v>
@@ -2659,7 +2697,7 @@
         <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>86</v>
+        <v>254</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>126</v>
@@ -2742,7 +2780,7 @@
         <v>138</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>87</v>
+        <v>255</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>125</v>
@@ -2825,7 +2863,7 @@
         <v>139</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>88</v>
+        <v>256</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>125</v>
@@ -2908,7 +2946,7 @@
         <v>140</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>125</v>
@@ -2991,7 +3029,7 @@
         <v>141</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>125</v>
@@ -3074,7 +3112,7 @@
         <v>140</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>91</v>
+        <v>259</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>125</v>
@@ -3157,7 +3195,7 @@
         <v>158</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>92</v>
+        <v>252</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>125</v>
@@ -3240,7 +3278,7 @@
         <v>158</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>93</v>
+        <v>254</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>125</v>
@@ -3323,7 +3361,7 @@
         <v>158</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>94</v>
+        <v>255</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>125</v>
@@ -3406,7 +3444,7 @@
         <v>159</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>95</v>
+        <v>256</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>125</v>
@@ -3489,7 +3527,7 @@
         <v>159</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>96</v>
+        <v>257</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>125</v>
@@ -3572,7 +3610,7 @@
         <v>159</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>97</v>
+        <v>258</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>125</v>
@@ -3655,7 +3693,7 @@
         <v>71</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>125</v>
@@ -3738,7 +3776,7 @@
         <v>71</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>125</v>
@@ -3821,7 +3859,7 @@
         <v>71</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>100</v>
+        <v>254</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>125</v>
@@ -3904,7 +3942,7 @@
         <v>71</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>101</v>
+        <v>255</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>125</v>
@@ -3987,7 +4025,7 @@
         <v>71</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>102</v>
+        <v>256</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>125</v>
@@ -4070,7 +4108,7 @@
         <v>71</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>103</v>
+        <v>257</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>125</v>
@@ -4153,7 +4191,7 @@
         <v>71</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>104</v>
+        <v>258</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>125</v>
@@ -4236,7 +4274,7 @@
         <v>71</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>105</v>
+        <v>259</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>125</v>
@@ -4319,7 +4357,7 @@
         <v>71</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>106</v>
+        <v>252</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>125</v>
@@ -4402,7 +4440,7 @@
         <v>71</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>107</v>
+        <v>254</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>125</v>
@@ -4485,7 +4523,7 @@
         <v>71</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>125</v>
@@ -4568,7 +4606,7 @@
         <v>71</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>109</v>
+        <v>256</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>125</v>
@@ -4648,7 +4686,7 @@
         <v>242</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>126</v>
@@ -4722,7 +4760,7 @@
         <v>242</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>126</v>
@@ -4796,7 +4834,7 @@
         <v>242</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>126</v>
@@ -4870,7 +4908,7 @@
         <v>242</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
#32 #33 add teacher_newcomer_list and get honor
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323D8BB7-D45E-466A-93A7-5631D50DFEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEE745C-AC7E-714B-B8E2-053040C5898E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="30735" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30740" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="268">
   <si>
     <t>username</t>
   </si>
@@ -908,6 +908,36 @@
   </si>
   <si>
     <t>2022-5-7 00:00:05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s4 few well</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacher feel good</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>st_of_te</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:04</t>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:37</t>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:36</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -915,7 +945,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1312,41 +1342,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="207" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="4"/>
+    <col min="9" max="9" width="8.83203125" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="4"/>
-    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.875" style="4"/>
+    <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.83203125" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1462,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
@@ -1515,7 +1545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
         <v>110</v>
       </c>
@@ -1598,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
@@ -1681,7 +1711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -1764,7 +1794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -1847,7 +1877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
         <v>114</v>
       </c>
@@ -1930,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
         <v>115</v>
       </c>
@@ -2013,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
         <v>116</v>
       </c>
@@ -2096,7 +2126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
         <v>117</v>
       </c>
@@ -2179,7 +2209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
         <v>118</v>
       </c>
@@ -2262,7 +2292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28">
       <c r="A12" s="4" t="s">
         <v>119</v>
       </c>
@@ -2345,7 +2375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28">
       <c r="A13" s="4" t="s">
         <v>120</v>
       </c>
@@ -2428,7 +2458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28">
       <c r="A14" s="4" t="s">
         <v>121</v>
       </c>
@@ -2511,7 +2541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28">
       <c r="A15" s="4" t="s">
         <v>122</v>
       </c>
@@ -2594,7 +2624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28">
       <c r="A16" s="4" t="s">
         <v>123</v>
       </c>
@@ -2677,7 +2707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28">
       <c r="A17" s="4" t="s">
         <v>124</v>
       </c>
@@ -2760,7 +2790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28">
       <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
@@ -2843,7 +2873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
@@ -2926,7 +2956,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28">
       <c r="A20" s="4" t="s">
         <v>133</v>
       </c>
@@ -3009,7 +3039,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28">
       <c r="A21" s="4" t="s">
         <v>135</v>
       </c>
@@ -3092,7 +3122,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28">
       <c r="A22" s="4" t="s">
         <v>137</v>
       </c>
@@ -3175,7 +3205,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28">
       <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
@@ -3258,7 +3288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28">
       <c r="A24" s="4" t="s">
         <v>149</v>
       </c>
@@ -3341,7 +3371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28">
       <c r="A25" s="4" t="s">
         <v>151</v>
       </c>
@@ -3424,7 +3454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28">
       <c r="A26" s="4" t="s">
         <v>153</v>
       </c>
@@ -3507,7 +3537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -3590,7 +3620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28">
       <c r="A28" s="4" t="s">
         <v>157</v>
       </c>
@@ -3673,7 +3703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28">
       <c r="A29" s="4" t="s">
         <v>196</v>
       </c>
@@ -3756,7 +3786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28">
       <c r="A30" s="4" t="s">
         <v>197</v>
       </c>
@@ -3839,7 +3869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28">
       <c r="A31" s="4" t="s">
         <v>198</v>
       </c>
@@ -3922,7 +3952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28">
       <c r="A32" s="4" t="s">
         <v>199</v>
       </c>
@@ -4005,7 +4035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28">
       <c r="A33" s="4" t="s">
         <v>200</v>
       </c>
@@ -4088,7 +4118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28">
       <c r="A34" s="4" t="s">
         <v>201</v>
       </c>
@@ -4171,7 +4201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28">
       <c r="A35" s="4" t="s">
         <v>202</v>
       </c>
@@ -4254,7 +4284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28">
       <c r="A36" s="4" t="s">
         <v>203</v>
       </c>
@@ -4337,7 +4367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28">
       <c r="A37" s="4" t="s">
         <v>204</v>
       </c>
@@ -4420,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28">
       <c r="A38" s="4" t="s">
         <v>205</v>
       </c>
@@ -4503,7 +4533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28">
       <c r="A39" s="4" t="s">
         <v>206</v>
       </c>
@@ -4586,7 +4616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28">
       <c r="A40" s="4" t="s">
         <v>207</v>
       </c>
@@ -4669,7 +4699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4743,7 +4773,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28">
       <c r="A42" s="4" t="s">
         <v>239</v>
       </c>
@@ -4817,7 +4847,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28">
       <c r="A43" s="4" t="s">
         <v>240</v>
       </c>
@@ -4891,7 +4921,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28">
       <c r="A44" s="4" t="s">
         <v>241</v>
       </c>
@@ -4953,7 +4983,7 @@
         <v>77</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="Z44" s="4" t="s">
         <v>77</v>
@@ -4963,6 +4993,83 @@
       </c>
       <c r="AB44" s="4" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
+      <c r="A45" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="R45" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="S45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="T45" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="U45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="W45" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="X45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y45" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="Z45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA45" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB45" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -5011,9 +5118,10 @@
     <hyperlink ref="B43" r:id="rId41" xr:uid="{6BDE2B2B-396F-9646-A14A-A47A4CBDF0FD}"/>
     <hyperlink ref="B40" r:id="rId42" xr:uid="{9BE6E5DB-9ED5-D445-A82F-149B56DE779C}"/>
     <hyperlink ref="B44" r:id="rId43" xr:uid="{3DA1C4FE-DC71-3647-B52C-E065CA59C3B0}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{21C402C8-23D4-EA4C-B714-A7D2D4F747F0}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
 
@@ -5025,14 +5133,14 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5061,7 +5169,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5090,7 +5198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5116,7 +5224,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5142,7 +5250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5168,7 +5276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5194,7 +5302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5220,7 +5328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5246,7 +5354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5272,7 +5380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5298,7 +5406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5324,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5364,21 +5472,21 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
-    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5413,7 +5521,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5448,7 +5556,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5483,7 +5591,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5518,7 +5626,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5553,7 +5661,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5588,7 +5696,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5623,7 +5731,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5658,7 +5766,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5693,7 +5801,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5728,7 +5836,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5763,7 +5871,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5798,7 +5906,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12">
       <c r="B13" s="7" t="s">
         <v>128</v>
       </c>
@@ -5833,7 +5941,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12">
       <c r="B14" s="7" t="s">
         <v>130</v>
       </c>
@@ -5868,7 +5976,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12">
       <c r="B15" s="7" t="s">
         <v>132</v>
       </c>
@@ -5903,7 +6011,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12">
       <c r="B16" s="7" t="s">
         <v>134</v>
       </c>
@@ -5938,7 +6046,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:12">
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
@@ -5973,7 +6081,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:12">
       <c r="B18" s="7" t="s">
         <v>146</v>
       </c>
@@ -6008,7 +6116,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:12">
       <c r="B19" s="7" t="s">
         <v>148</v>
       </c>
@@ -6043,7 +6151,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12">
       <c r="B20" s="7" t="s">
         <v>150</v>
       </c>
@@ -6078,7 +6186,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:12">
       <c r="B21" s="7" t="s">
         <v>152</v>
       </c>
@@ -6113,7 +6221,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:12">
       <c r="B22" s="7" t="s">
         <v>154</v>
       </c>
@@ -6148,7 +6256,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12">
       <c r="B23" s="7" t="s">
         <v>156</v>
       </c>
@@ -6197,12 +6305,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6219,7 +6327,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -6250,9 +6358,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6266,7 +6374,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="C2" t="s">
         <v>129</v>
       </c>
@@ -6274,7 +6382,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="C3" t="s">
         <v>129</v>
       </c>
@@ -6282,7 +6390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="C4" t="s">
         <v>129</v>
       </c>
@@ -6298,22 +6406,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:G4"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="295" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="295" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6333,7 +6441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" t="s">
         <v>129</v>
       </c>
@@ -6353,7 +6461,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>130</v>
       </c>
@@ -6373,7 +6481,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>132</v>
       </c>
@@ -6391,6 +6499,46 @@
       </c>
       <c r="G4" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -6407,13 +6555,13 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -6427,7 +6575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>171</v>
       </c>
@@ -6441,7 +6589,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>172</v>
       </c>
@@ -6455,7 +6603,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>173</v>
       </c>
@@ -6469,7 +6617,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>174</v>
       </c>
@@ -6483,7 +6631,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>175</v>
       </c>
@@ -6497,7 +6645,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>176</v>
       </c>
@@ -6525,18 +6673,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="4" width="8.875" style="4"/>
+    <col min="1" max="4" width="8.83203125" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="4"/>
-    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>183</v>
       </c>
@@ -6568,7 +6716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6597,7 +6745,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6640,17 +6788,17 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="4"/>
+    <col min="14" max="15" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -6706,7 +6854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6750,7 +6898,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6794,7 +6942,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6838,7 +6986,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6896,15 +7044,15 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -6930,7 +7078,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6953,7 +7101,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6990,12 +7138,12 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -7018,7 +7166,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7055,12 +7203,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -7071,7 +7219,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
         <v>126</v>
       </c>
@@ -7082,7 +7230,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
         <v>126</v>
       </c>
@@ -7093,7 +7241,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="B4" s="4" t="s">
         <v>144</v>
       </c>
@@ -7104,7 +7252,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4">
       <c r="B5" s="4" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
#33 now honor is work well with frontend
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEE745C-AC7E-714B-B8E2-053040C5898E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F290A87-FE4A-5C43-96FB-B64224E5C2F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="30740" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="30740" windowHeight="15160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="271">
   <si>
     <t>username</t>
   </si>
@@ -938,6 +938,18 @@
   </si>
   <si>
     <t>2020-12-12 00:00:36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>认真</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>负责</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能干</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1344,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G29" zoomScale="207" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="207" workbookViewId="0">
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
@@ -6352,10 +6364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:E4"/>
+  <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="340" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -6375,6 +6387,9 @@
       </c>
     </row>
     <row r="2" spans="2:5">
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
         <v>129</v>
       </c>
@@ -6383,6 +6398,9 @@
       </c>
     </row>
     <row r="3" spans="2:5">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
         <v>129</v>
       </c>
@@ -6391,11 +6409,47 @@
       </c>
     </row>
     <row r="4" spans="2:5">
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>129</v>
       </c>
       <c r="E4" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#34 #35 Fixed unit test for starting and ending exams
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F290A87-FE4A-5C43-96FB-B64224E5C2F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFA693E-0595-4F25-A05D-60F0188D5F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="30740" windowHeight="15160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="274">
   <si>
     <t>username</t>
   </si>
@@ -950,6 +950,18 @@
   </si>
   <si>
     <t>能干</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -957,7 +969,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1037,7 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1051,6 +1063,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1360,35 +1373,35 @@
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="8.875" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.83203125" style="4"/>
-    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.83203125" style="4"/>
+    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.875" style="4"/>
+    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
@@ -1557,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>110</v>
       </c>
@@ -1640,7 +1653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
@@ -1723,7 +1736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -1806,7 +1819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -1889,7 +1902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>114</v>
       </c>
@@ -1972,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>115</v>
       </c>
@@ -2055,7 +2068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>116</v>
       </c>
@@ -2138,7 +2151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>117</v>
       </c>
@@ -2221,7 +2234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>118</v>
       </c>
@@ -2304,7 +2317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>119</v>
       </c>
@@ -2387,7 +2400,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>120</v>
       </c>
@@ -2470,7 +2483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>121</v>
       </c>
@@ -2553,7 +2566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>122</v>
       </c>
@@ -2636,7 +2649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>123</v>
       </c>
@@ -2719,7 +2732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>124</v>
       </c>
@@ -2802,7 +2815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
@@ -2885,7 +2898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
@@ -2968,7 +2981,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>133</v>
       </c>
@@ -3051,7 +3064,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>135</v>
       </c>
@@ -3134,7 +3147,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>137</v>
       </c>
@@ -3217,7 +3230,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
@@ -3300,7 +3313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>149</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>151</v>
       </c>
@@ -3466,7 +3479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>153</v>
       </c>
@@ -3549,7 +3562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -3632,7 +3645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>157</v>
       </c>
@@ -3715,7 +3728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>196</v>
       </c>
@@ -3798,7 +3811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>197</v>
       </c>
@@ -3881,7 +3894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>198</v>
       </c>
@@ -3964,7 +3977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>199</v>
       </c>
@@ -4047,7 +4060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>200</v>
       </c>
@@ -4130,7 +4143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>201</v>
       </c>
@@ -4213,7 +4226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>202</v>
       </c>
@@ -4296,7 +4309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>203</v>
       </c>
@@ -4379,7 +4392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>204</v>
       </c>
@@ -4462,7 +4475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>205</v>
       </c>
@@ -4545,7 +4558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>206</v>
       </c>
@@ -4628,7 +4641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>207</v>
       </c>
@@ -4711,7 +4724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4785,7 +4798,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>239</v>
       </c>
@@ -4859,7 +4872,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>240</v>
       </c>
@@ -4933,7 +4946,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>241</v>
       </c>
@@ -5007,7 +5020,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>262</v>
       </c>
@@ -5145,14 +5158,14 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1">
+    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5181,7 +5194,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5210,7 +5223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5236,7 +5249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5262,7 +5275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5288,7 +5301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5314,7 +5327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5340,7 +5353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5366,7 +5379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5392,7 +5405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5418,7 +5431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5444,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5478,27 +5491,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L23"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="221" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="221" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4"/>
-    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1">
+    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5533,7 +5546,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5568,7 +5581,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5603,7 +5616,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5638,7 +5651,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5673,7 +5686,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5708,7 +5721,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5743,7 +5756,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5778,7 +5791,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5813,7 +5826,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5848,7 +5861,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5883,7 +5896,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5918,7 +5931,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B13" s="7" t="s">
         <v>128</v>
       </c>
@@ -5953,7 +5966,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B14" s="7" t="s">
         <v>130</v>
       </c>
@@ -5988,7 +6001,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B15" s="7" t="s">
         <v>132</v>
       </c>
@@ -6023,7 +6036,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B16" s="7" t="s">
         <v>134</v>
       </c>
@@ -6058,7 +6071,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
@@ -6093,7 +6106,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B18" s="7" t="s">
         <v>146</v>
       </c>
@@ -6128,7 +6141,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
         <v>148</v>
       </c>
@@ -6163,7 +6176,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B20" s="7" t="s">
         <v>150</v>
       </c>
@@ -6198,7 +6211,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B21" s="7" t="s">
         <v>152</v>
       </c>
@@ -6233,7 +6246,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B22" s="7" t="s">
         <v>154</v>
       </c>
@@ -6268,7 +6281,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B23" s="7" t="s">
         <v>156</v>
       </c>
@@ -6279,13 +6292,13 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>104</v>
+        <v>271</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>104</v>
+        <v>271</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>104</v>
+        <v>271</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>68</v>
@@ -6301,6 +6314,41 @@
       </c>
       <c r="L23" s="4" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -6317,12 +6365,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1">
+    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6339,7 +6387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -6366,13 +6414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+    <sheetView zoomScale="189" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6386,7 +6434,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6397,7 +6445,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6408,7 +6456,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>2</v>
       </c>
@@ -6419,7 +6467,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>0</v>
       </c>
@@ -6430,7 +6478,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6441,7 +6489,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>2</v>
       </c>
@@ -6466,16 +6514,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6495,7 +6543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>129</v>
       </c>
@@ -6515,7 +6563,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>130</v>
       </c>
@@ -6535,7 +6583,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>132</v>
       </c>
@@ -6555,7 +6603,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>240</v>
       </c>
@@ -6575,7 +6623,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>240</v>
       </c>
@@ -6609,13 +6657,13 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -6629,7 +6677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>171</v>
       </c>
@@ -6643,7 +6691,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>172</v>
       </c>
@@ -6657,7 +6705,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>173</v>
       </c>
@@ -6671,7 +6719,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>174</v>
       </c>
@@ -6685,7 +6733,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>175</v>
       </c>
@@ -6699,7 +6747,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>176</v>
       </c>
@@ -6727,18 +6775,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="4"/>
+    <col min="1" max="4" width="8.875" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="4"/>
-    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.875" style="4"/>
+    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>183</v>
       </c>
@@ -6770,7 +6818,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6799,7 +6847,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6838,21 +6886,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView zoomScale="214" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.83203125" style="4"/>
+    <col min="14" max="15" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -6908,7 +6956,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6952,7 +7000,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6996,7 +7044,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7040,7 +7088,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7098,15 +7146,15 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -7132,7 +7180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7155,7 +7203,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7192,12 +7240,12 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -7220,7 +7268,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7257,12 +7305,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1">
+    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -7273,7 +7321,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>126</v>
       </c>
@@ -7284,7 +7332,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>126</v>
       </c>
@@ -7295,7 +7343,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>144</v>
       </c>
@@ -7306,7 +7354,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
#35 #36 Added API for marking a task as finished, as well as related unit tests
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFA693E-0595-4F25-A05D-60F0188D5F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F82EBE1-8D99-48E9-BFCA-8833DCA9603E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="275">
   <si>
     <t>username</t>
   </si>
@@ -962,6 +962,10 @@
   </si>
   <si>
     <t>25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5491,10 +5495,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L24"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="221" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6348,7 +6352,42 @@
         <v>272</v>
       </c>
       <c r="L24" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>273</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases, fixed bugs
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F82EBE1-8D99-48E9-BFCA-8833DCA9603E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AB81E0-FBE2-4CBD-B1C7-CE61FB30DB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="285">
   <si>
     <t>username</t>
   </si>
@@ -966,6 +966,45 @@
   </si>
   <si>
     <t>23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>questions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.\files\test\admin_c_1651157940.0784883\SampleTestPaper_admin_ex_1651157940.0784883.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020-12-12 00:00:00</t>
+  </si>
+  <si>
+    <t>样例2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.\files\test\admin_c_1651198092.9064405\SampleTest2_admin_ex_1651198092.9064405.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>样例3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.\files\test\test_content_exam_1\sample3.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>27</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -973,7 +1012,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1016,6 +1055,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1053,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1068,6 +1116,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1377,35 +1426,35 @@
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="7.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="4"/>
+    <col min="9" max="9" width="8.88671875" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="4"/>
-    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.875" style="4"/>
+    <col min="12" max="12" width="21.88671875" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.88671875" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.88671875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.109375" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.88671875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
@@ -1574,7 +1623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>110</v>
       </c>
@@ -1657,7 +1706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
@@ -1740,7 +1789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -1823,7 +1872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -1906,7 +1955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>114</v>
       </c>
@@ -1989,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>115</v>
       </c>
@@ -2072,7 +2121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>116</v>
       </c>
@@ -2155,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>117</v>
       </c>
@@ -2238,7 +2287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>118</v>
       </c>
@@ -2321,7 +2370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>119</v>
       </c>
@@ -2404,7 +2453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>120</v>
       </c>
@@ -2487,7 +2536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>121</v>
       </c>
@@ -2570,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>122</v>
       </c>
@@ -2653,7 +2702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>123</v>
       </c>
@@ -2736,7 +2785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>124</v>
       </c>
@@ -2819,7 +2868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>129</v>
       </c>
@@ -2902,7 +2951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>131</v>
       </c>
@@ -2985,7 +3034,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>133</v>
       </c>
@@ -3068,7 +3117,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>135</v>
       </c>
@@ -3151,7 +3200,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>137</v>
       </c>
@@ -3234,7 +3283,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
@@ -3317,7 +3366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>149</v>
       </c>
@@ -3400,7 +3449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>151</v>
       </c>
@@ -3483,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>153</v>
       </c>
@@ -3566,7 +3615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>155</v>
       </c>
@@ -3649,7 +3698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>157</v>
       </c>
@@ -3732,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>196</v>
       </c>
@@ -3815,7 +3864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>197</v>
       </c>
@@ -3898,7 +3947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>198</v>
       </c>
@@ -3981,7 +4030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>199</v>
       </c>
@@ -4064,7 +4113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>200</v>
       </c>
@@ -4147,7 +4196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>201</v>
       </c>
@@ -4230,7 +4279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>202</v>
       </c>
@@ -4313,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>203</v>
       </c>
@@ -4396,7 +4445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>204</v>
       </c>
@@ -4479,7 +4528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>205</v>
       </c>
@@ -4562,7 +4611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>206</v>
       </c>
@@ -4645,7 +4694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>207</v>
       </c>
@@ -4728,7 +4777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4802,7 +4851,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>239</v>
       </c>
@@ -4876,7 +4925,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>240</v>
       </c>
@@ -4950,7 +4999,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>241</v>
       </c>
@@ -5024,7 +5073,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>262</v>
       </c>
@@ -5162,14 +5211,14 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5198,7 +5247,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5227,7 +5276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5253,7 +5302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5279,7 +5328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5305,7 +5354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5331,7 +5380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5357,7 +5406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5383,7 +5432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5409,7 +5458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5435,7 +5484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5461,7 +5510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5495,27 +5544,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="221" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
-    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="7.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5550,7 +5599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -5585,7 +5634,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>131</v>
       </c>
@@ -5620,7 +5669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>133</v>
       </c>
@@ -5655,7 +5704,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>135</v>
       </c>
@@ -5690,7 +5739,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>137</v>
       </c>
@@ -5725,7 +5774,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>147</v>
       </c>
@@ -5760,7 +5809,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>149</v>
       </c>
@@ -5795,7 +5844,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>151</v>
       </c>
@@ -5830,7 +5879,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>153</v>
       </c>
@@ -5865,7 +5914,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>155</v>
       </c>
@@ -5900,7 +5949,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
@@ -5935,7 +5984,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>128</v>
       </c>
@@ -5970,7 +6019,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>130</v>
       </c>
@@ -6005,7 +6054,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>132</v>
       </c>
@@ -6040,7 +6089,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>134</v>
       </c>
@@ -6075,7 +6124,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>136</v>
       </c>
@@ -6110,7 +6159,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>146</v>
       </c>
@@ -6145,7 +6194,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>148</v>
       </c>
@@ -6180,7 +6229,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>150</v>
       </c>
@@ -6215,7 +6264,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>152</v>
       </c>
@@ -6250,7 +6299,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>154</v>
       </c>
@@ -6285,7 +6334,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>156</v>
       </c>
@@ -6320,7 +6369,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>240</v>
       </c>
@@ -6355,18 +6404,18 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>241</v>
       </c>
       <c r="C25" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="9">
         <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>104</v>
+        <v>271</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>104</v>
@@ -6388,6 +6437,76 @@
       </c>
       <c r="L25" s="4" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -6404,12 +6523,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6426,7 +6545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>129</v>
       </c>
@@ -6457,9 +6576,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6473,7 +6592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6484,7 +6603,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6495,7 +6614,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -6506,7 +6625,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0</v>
       </c>
@@ -6517,7 +6636,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6528,7 +6647,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -6553,16 +6672,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6582,7 +6701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>129</v>
       </c>
@@ -6602,7 +6721,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>130</v>
       </c>
@@ -6622,7 +6741,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>132</v>
       </c>
@@ -6642,7 +6761,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>240</v>
       </c>
@@ -6662,7 +6781,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>240</v>
       </c>
@@ -6696,13 +6815,13 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -6716,7 +6835,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>171</v>
       </c>
@@ -6730,7 +6849,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>172</v>
       </c>
@@ -6744,7 +6863,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>173</v>
       </c>
@@ -6758,7 +6877,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>174</v>
       </c>
@@ -6772,7 +6891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>175</v>
       </c>
@@ -6786,7 +6905,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>176</v>
       </c>
@@ -6814,18 +6933,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.875" style="4"/>
+    <col min="1" max="4" width="8.88671875" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="4"/>
-    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>183</v>
       </c>
@@ -6857,7 +6976,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6886,7 +7005,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6923,23 +7042,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
-    <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="4"/>
+    <col min="14" max="15" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -6994,8 +7113,11 @@
       <c r="R1" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S1" s="10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7039,7 +7161,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7082,8 +7204,11 @@
       <c r="Q3" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S3" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7127,7 +7252,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7159,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>83</v>
@@ -7169,6 +7294,100 @@
       </c>
       <c r="Q5" s="4" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="S6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="S7" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -7185,15 +7404,15 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -7219,7 +7438,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7242,7 +7461,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7279,12 +7498,12 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -7307,7 +7526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7344,12 +7563,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -7360,7 +7579,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>126</v>
       </c>
@@ -7371,7 +7590,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>126</v>
       </c>
@@ -7382,7 +7601,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>144</v>
       </c>
@@ -7393,7 +7612,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
#38 change unit-test data to beautify
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D006E87-311B-45B7-98BC-7314885FAB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE4547D-60E3-42B6-B63C-30CA580B6737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="4290" windowWidth="30735" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -847,18 +847,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2020-12-12 00:00:33</t>
-  </si>
-  <si>
-    <t>2020-12-12 00:00:34</t>
-  </si>
-  <si>
-    <t>2020-12-12 00:00:35</t>
-  </si>
-  <si>
-    <t>2020-12-12 00:00:36</t>
-  </si>
-  <si>
     <t>admin13</t>
   </si>
   <si>
@@ -930,13 +918,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2020-12-12 00:00:37</t>
-  </si>
-  <si>
-    <t>2020-12-12 00:00:36</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>认真</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -949,10 +930,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2020-12-12 00:00:27</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>24</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1075,6 +1052,32 @@
   </si>
   <si>
     <t>策划部门</t>
+  </si>
+  <si>
+    <t>2022-5-2 00:00:06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-2 00:00:08</t>
+  </si>
+  <si>
+    <t>2022-5-2 00:00:10</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-4 00:00:06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1491,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E49" sqref="E46:E49"/>
+    <sheetView topLeftCell="T1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27:W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1579,7 +1582,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="T1" s="3" t="s">
         <v>18</v>
@@ -1623,13 +1626,13 @@
         <v>70</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I2" s="4">
         <v>1</v>
@@ -1659,13 +1662,13 @@
         <v>76</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="U2" s="4">
         <v>0</v>
@@ -1674,19 +1677,19 @@
         <v>0</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>73</v>
+        <v>246</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>73</v>
+        <v>292</v>
       </c>
       <c r="Z2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>73</v>
+        <v>292</v>
       </c>
       <c r="AB2" s="4">
         <v>5</v>
@@ -1706,13 +1709,13 @@
         <v>70</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
@@ -1742,13 +1745,13 @@
         <v>1</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="U3" s="4">
         <v>0</v>
@@ -1757,19 +1760,19 @@
         <v>0</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>73</v>
+        <v>251</v>
       </c>
       <c r="X3" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>73</v>
+        <v>293</v>
       </c>
       <c r="Z3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>73</v>
+        <v>293</v>
       </c>
       <c r="AB3" s="4">
         <v>5</v>
@@ -1789,13 +1792,13 @@
         <v>70</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I4" s="4">
         <v>1</v>
@@ -1810,7 +1813,7 @@
         <v>73</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>76</v>
@@ -1825,13 +1828,13 @@
         <v>76</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="U4" s="4">
         <v>0</v>
@@ -1840,19 +1843,19 @@
         <v>0</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>73</v>
+        <v>252</v>
       </c>
       <c r="X4" s="4">
         <v>1</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>73</v>
+        <v>294</v>
       </c>
       <c r="Z4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>73</v>
+        <v>294</v>
       </c>
       <c r="AB4" s="4">
         <v>5</v>
@@ -1872,13 +1875,13 @@
         <v>70</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I5" s="4">
         <v>1</v>
@@ -1908,13 +1911,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="U5" s="4">
         <v>0</v>
@@ -1923,19 +1926,19 @@
         <v>0</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>73</v>
+        <v>295</v>
       </c>
       <c r="Z5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>73</v>
+        <v>295</v>
       </c>
       <c r="AB5" s="4">
         <v>5</v>
@@ -1955,13 +1958,13 @@
         <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
@@ -1991,13 +1994,13 @@
         <v>76</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>76</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="U6" s="4">
         <v>0</v>
@@ -2006,19 +2009,19 @@
         <v>0</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>73</v>
+        <v>249</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>73</v>
+        <v>286</v>
       </c>
       <c r="Z6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>73</v>
+        <v>286</v>
       </c>
       <c r="AB6" s="4">
         <v>5</v>
@@ -2038,13 +2041,13 @@
         <v>70</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I7" s="4">
         <v>1</v>
@@ -2074,13 +2077,13 @@
         <v>125</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="U7" s="4">
         <v>0</v>
@@ -2089,19 +2092,19 @@
         <v>0</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="Z7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="AB7" s="4">
         <v>5</v>
@@ -2121,13 +2124,13 @@
         <v>70</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I8" s="4">
         <v>1</v>
@@ -2142,7 +2145,7 @@
         <v>73</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>76</v>
@@ -2157,13 +2160,13 @@
         <v>76</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="U8" s="4">
         <v>0</v>
@@ -2172,19 +2175,19 @@
         <v>0</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>73</v>
+        <v>246</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>73</v>
+        <v>288</v>
       </c>
       <c r="Z8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>73</v>
+        <v>288</v>
       </c>
       <c r="AB8" s="4">
         <v>5</v>
@@ -2204,13 +2207,13 @@
         <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>125</v>
@@ -2240,13 +2243,13 @@
         <v>125</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>76</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="U9" s="4">
         <v>0</v>
@@ -2255,19 +2258,19 @@
         <v>0</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>77</v>
+        <v>278</v>
       </c>
       <c r="Z9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>77</v>
+        <v>278</v>
       </c>
       <c r="AB9" s="4">
         <v>5</v>
@@ -2287,13 +2290,13 @@
         <v>70</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>125</v>
@@ -2323,13 +2326,13 @@
         <v>76</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="U10" s="4">
         <v>0</v>
@@ -2338,19 +2341,19 @@
         <v>0</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>78</v>
+        <v>248</v>
       </c>
       <c r="X10" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>78</v>
+        <v>279</v>
       </c>
       <c r="Z10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>78</v>
+        <v>279</v>
       </c>
       <c r="AB10" s="4">
         <v>5</v>
@@ -2370,13 +2373,13 @@
         <v>70</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>125</v>
@@ -2406,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="U11" s="4">
         <v>0</v>
@@ -2421,19 +2424,19 @@
         <v>0</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>79</v>
+        <v>247</v>
       </c>
       <c r="X11" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>79</v>
+        <v>280</v>
       </c>
       <c r="Z11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>79</v>
+        <v>280</v>
       </c>
       <c r="AB11" s="4">
         <v>5</v>
@@ -2453,13 +2456,13 @@
         <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>125</v>
@@ -2474,7 +2477,7 @@
         <v>80</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N12" s="4">
         <v>1</v>
@@ -2489,13 +2492,13 @@
         <v>76</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="U12" s="4">
         <v>0</v>
@@ -2504,19 +2507,19 @@
         <v>0</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="X12" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>80</v>
+        <v>281</v>
       </c>
       <c r="Z12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>80</v>
+        <v>281</v>
       </c>
       <c r="AB12" s="4">
         <v>5</v>
@@ -2536,13 +2539,13 @@
         <v>70</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>125</v>
@@ -2572,13 +2575,13 @@
         <v>1</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="U13" s="4">
         <v>0</v>
@@ -2587,19 +2590,19 @@
         <v>0</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>81</v>
+        <v>250</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>81</v>
+        <v>282</v>
       </c>
       <c r="Z13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>81</v>
+        <v>282</v>
       </c>
       <c r="AB13" s="4">
         <v>5</v>
@@ -2619,13 +2622,13 @@
         <v>70</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>125</v>
@@ -2655,13 +2658,13 @@
         <v>76</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="U14" s="4">
         <v>0</v>
@@ -2670,19 +2673,19 @@
         <v>0</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>82</v>
+        <v>248</v>
       </c>
       <c r="X14" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>82</v>
+        <v>283</v>
       </c>
       <c r="Z14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>82</v>
+        <v>283</v>
       </c>
       <c r="AB14" s="4">
         <v>5</v>
@@ -2702,13 +2705,13 @@
         <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>125</v>
@@ -2738,13 +2741,13 @@
         <v>1</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="U15" s="4">
         <v>0</v>
@@ -2753,19 +2756,19 @@
         <v>0</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>83</v>
+        <v>248</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>83</v>
+        <v>284</v>
       </c>
       <c r="Z15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>83</v>
+        <v>284</v>
       </c>
       <c r="AB15" s="4">
         <v>5</v>
@@ -2785,13 +2788,13 @@
         <v>70</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>125</v>
@@ -2806,7 +2809,7 @@
         <v>84</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N16" s="4">
         <v>1</v>
@@ -2821,13 +2824,13 @@
         <v>76</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="U16" s="4">
         <v>0</v>
@@ -2836,19 +2839,19 @@
         <v>0</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>84</v>
+        <v>252</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>84</v>
+        <v>285</v>
       </c>
       <c r="Z16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>84</v>
+        <v>285</v>
       </c>
       <c r="AB16" s="4">
         <v>5</v>
@@ -2868,13 +2871,13 @@
         <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>125</v>
@@ -2904,13 +2907,13 @@
         <v>1</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S17" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="U17" s="4">
         <v>0</v>
@@ -2919,19 +2922,19 @@
         <v>0</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="X17" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>85</v>
+        <v>296</v>
       </c>
       <c r="Z17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>85</v>
+        <v>296</v>
       </c>
       <c r="AB17" s="4">
         <v>5</v>
@@ -2951,13 +2954,13 @@
         <v>70</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>137</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>124</v>
@@ -2987,13 +2990,13 @@
         <v>1</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>75</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="U18" s="4">
         <v>0</v>
@@ -3002,19 +3005,19 @@
         <v>0</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="X18" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>86</v>
+        <v>289</v>
       </c>
       <c r="Z18" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>86</v>
+        <v>289</v>
       </c>
       <c r="AB18" s="4">
         <v>5</v>
@@ -3034,13 +3037,13 @@
         <v>70</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>138</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>124</v>
@@ -3070,13 +3073,13 @@
         <v>1</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U19" s="4">
         <v>0</v>
@@ -3085,19 +3088,19 @@
         <v>0</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>87</v>
+        <v>251</v>
       </c>
       <c r="X19" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>87</v>
+        <v>277</v>
       </c>
       <c r="Z19" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>87</v>
+        <v>277</v>
       </c>
       <c r="AB19" s="4" t="s">
         <v>144</v>
@@ -3117,13 +3120,13 @@
         <v>70</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>139</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>124</v>
@@ -3138,7 +3141,7 @@
         <v>88</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>75</v>
@@ -3153,13 +3156,13 @@
         <v>1</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S20" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U20" s="4">
         <v>0</v>
@@ -3168,19 +3171,19 @@
         <v>0</v>
       </c>
       <c r="W20" s="4" t="s">
-        <v>88</v>
+        <v>252</v>
       </c>
       <c r="X20" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>88</v>
+        <v>277</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>88</v>
+        <v>277</v>
       </c>
       <c r="AB20" s="4" t="s">
         <v>144</v>
@@ -3200,13 +3203,13 @@
         <v>70</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>140</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>124</v>
@@ -3236,13 +3239,13 @@
         <v>1</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U21" s="4">
         <v>0</v>
@@ -3251,19 +3254,19 @@
         <v>0</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>89</v>
+        <v>251</v>
       </c>
       <c r="X21" s="4" t="s">
         <v>143</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>89</v>
+        <v>277</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA21" s="4" t="s">
-        <v>89</v>
+        <v>277</v>
       </c>
       <c r="AB21" s="4" t="s">
         <v>144</v>
@@ -3283,13 +3286,13 @@
         <v>70</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>139</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>124</v>
@@ -3319,13 +3322,13 @@
         <v>1</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="U22" s="4">
         <v>0</v>
@@ -3334,19 +3337,19 @@
         <v>0</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>90</v>
+        <v>251</v>
       </c>
       <c r="X22" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>90</v>
+        <v>290</v>
       </c>
       <c r="Z22" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>90</v>
+        <v>290</v>
       </c>
       <c r="AB22" s="4" t="s">
         <v>144</v>
@@ -3366,13 +3369,13 @@
         <v>70</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>124</v>
@@ -3402,13 +3405,13 @@
         <v>1</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U23" s="4">
         <v>0</v>
@@ -3417,19 +3420,19 @@
         <v>0</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="X23" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>91</v>
+        <v>277</v>
       </c>
       <c r="Z23" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>91</v>
+        <v>277</v>
       </c>
       <c r="AB23" s="4">
         <v>5</v>
@@ -3449,13 +3452,13 @@
         <v>70</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>124</v>
@@ -3470,7 +3473,7 @@
         <v>92</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>75</v>
@@ -3485,13 +3488,13 @@
         <v>1</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U24" s="4">
         <v>0</v>
@@ -3500,19 +3503,19 @@
         <v>0</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>92</v>
+        <v>251</v>
       </c>
       <c r="X24" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="Z24" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>92</v>
+        <v>277</v>
       </c>
       <c r="AB24" s="4">
         <v>5</v>
@@ -3532,13 +3535,13 @@
         <v>70</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>157</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>124</v>
@@ -3568,13 +3571,13 @@
         <v>1</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U25" s="4">
         <v>0</v>
@@ -3583,19 +3586,19 @@
         <v>0</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>93</v>
+        <v>252</v>
       </c>
       <c r="X25" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>93</v>
+        <v>277</v>
       </c>
       <c r="Z25" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA25" s="4" t="s">
-        <v>93</v>
+        <v>277</v>
       </c>
       <c r="AB25" s="4">
         <v>5</v>
@@ -3615,13 +3618,13 @@
         <v>70</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>158</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>124</v>
@@ -3651,13 +3654,13 @@
         <v>1</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U26" s="4">
         <v>0</v>
@@ -3666,19 +3669,19 @@
         <v>0</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>94</v>
+        <v>251</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="Z26" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="AB26" s="4">
         <v>5</v>
@@ -3698,13 +3701,13 @@
         <v>70</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>158</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>124</v>
@@ -3734,13 +3737,13 @@
         <v>1</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U27" s="4">
         <v>0</v>
@@ -3749,19 +3752,19 @@
         <v>0</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>95</v>
+        <v>251</v>
       </c>
       <c r="X27" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="Z27" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="AB27" s="4">
         <v>5</v>
@@ -3781,13 +3784,13 @@
         <v>70</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>158</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>124</v>
@@ -3802,7 +3805,7 @@
         <v>96</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>75</v>
@@ -3817,13 +3820,13 @@
         <v>1</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U28" s="4">
         <v>0</v>
@@ -3832,19 +3835,19 @@
         <v>0</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>96</v>
+        <v>252</v>
       </c>
       <c r="X28" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>96</v>
+        <v>277</v>
       </c>
       <c r="Z28" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>96</v>
+        <v>277</v>
       </c>
       <c r="AB28" s="4">
         <v>5</v>
@@ -3864,13 +3867,13 @@
         <v>70</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>124</v>
@@ -3900,13 +3903,13 @@
         <v>1</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U29" s="4">
         <v>0</v>
@@ -3915,19 +3918,19 @@
         <v>0</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>97</v>
+        <v>259</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>97</v>
+        <v>277</v>
       </c>
       <c r="Z29" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>97</v>
+        <v>277</v>
       </c>
       <c r="AB29" s="4">
         <v>5</v>
@@ -3947,13 +3950,13 @@
         <v>70</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>124</v>
@@ -3983,13 +3986,13 @@
         <v>1</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="U30" s="4">
         <v>0</v>
@@ -3998,19 +4001,19 @@
         <v>0</v>
       </c>
       <c r="W30" s="4" t="s">
-        <v>98</v>
+        <v>251</v>
       </c>
       <c r="X30" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>98</v>
+        <v>291</v>
       </c>
       <c r="Z30" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA30" s="4" t="s">
-        <v>98</v>
+        <v>291</v>
       </c>
       <c r="AB30" s="4">
         <v>5</v>
@@ -4030,13 +4033,13 @@
         <v>70</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>124</v>
@@ -4066,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U31" s="4">
         <v>0</v>
@@ -4081,19 +4084,19 @@
         <v>0</v>
       </c>
       <c r="W31" s="4" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="X31" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>99</v>
+        <v>277</v>
       </c>
       <c r="Z31" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA31" s="4" t="s">
-        <v>99</v>
+        <v>277</v>
       </c>
       <c r="AB31" s="4">
         <v>5</v>
@@ -4113,13 +4116,13 @@
         <v>70</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>124</v>
@@ -4134,7 +4137,7 @@
         <v>100</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>75</v>
@@ -4149,13 +4152,13 @@
         <v>1</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U32" s="4">
         <v>0</v>
@@ -4164,19 +4167,19 @@
         <v>0</v>
       </c>
       <c r="W32" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="X32" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>100</v>
+        <v>277</v>
       </c>
       <c r="Z32" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA32" s="4" t="s">
-        <v>100</v>
+        <v>277</v>
       </c>
       <c r="AB32" s="4">
         <v>5</v>
@@ -4196,13 +4199,13 @@
         <v>70</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>124</v>
@@ -4232,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>76</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U33" s="4">
         <v>0</v>
@@ -4247,19 +4250,19 @@
         <v>0</v>
       </c>
       <c r="W33" s="4" t="s">
-        <v>101</v>
+        <v>254</v>
       </c>
       <c r="X33" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="Z33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA33" s="4" t="s">
-        <v>101</v>
+        <v>277</v>
       </c>
       <c r="AB33" s="4">
         <v>5</v>
@@ -4279,13 +4282,13 @@
         <v>70</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>124</v>
@@ -4315,13 +4318,13 @@
         <v>1</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>125</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U34" s="4">
         <v>0</v>
@@ -4330,19 +4333,19 @@
         <v>0</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>102</v>
+        <v>253</v>
       </c>
       <c r="X34" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>102</v>
+        <v>277</v>
       </c>
       <c r="Z34" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA34" s="4" t="s">
-        <v>102</v>
+        <v>277</v>
       </c>
       <c r="AB34" s="4">
         <v>5</v>
@@ -4362,13 +4365,13 @@
         <v>70</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>124</v>
@@ -4398,13 +4401,13 @@
         <v>1</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U35" s="4">
         <v>0</v>
@@ -4413,19 +4416,19 @@
         <v>0</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>103</v>
+        <v>250</v>
       </c>
       <c r="X35" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="Z35" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="AB35" s="4">
         <v>5</v>
@@ -4445,13 +4448,13 @@
         <v>70</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>124</v>
@@ -4466,7 +4469,7 @@
         <v>104</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>75</v>
@@ -4481,13 +4484,13 @@
         <v>1</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>143</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="U36" s="4">
         <v>0</v>
@@ -4496,19 +4499,19 @@
         <v>0</v>
       </c>
       <c r="W36" s="4" t="s">
-        <v>104</v>
+        <v>246</v>
       </c>
       <c r="X36" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>104</v>
+        <v>286</v>
       </c>
       <c r="Z36" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA36" s="4" t="s">
-        <v>104</v>
+        <v>286</v>
       </c>
       <c r="AB36" s="4">
         <v>5</v>
@@ -4528,13 +4531,13 @@
         <v>70</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>124</v>
@@ -4564,34 +4567,34 @@
         <v>1</v>
       </c>
       <c r="R37" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S37" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="U37" s="4">
+        <v>0</v>
+      </c>
+      <c r="V37" s="4">
+        <v>0</v>
+      </c>
+      <c r="W37" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="T37" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="U37" s="4">
-        <v>0</v>
-      </c>
-      <c r="V37" s="4">
-        <v>0</v>
-      </c>
-      <c r="W37" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="X37" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>105</v>
+        <v>287</v>
       </c>
       <c r="Z37" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA37" s="4" t="s">
-        <v>105</v>
+        <v>287</v>
       </c>
       <c r="AB37" s="4">
         <v>5</v>
@@ -4611,13 +4614,13 @@
         <v>70</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>124</v>
@@ -4647,34 +4650,34 @@
         <v>1</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="S38" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="T38" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="U38" s="4">
+        <v>0</v>
+      </c>
+      <c r="V38" s="4">
+        <v>0</v>
+      </c>
+      <c r="W38" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="T38" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="U38" s="4">
-        <v>0</v>
-      </c>
-      <c r="V38" s="4">
-        <v>0</v>
-      </c>
-      <c r="W38" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="X38" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y38" s="4" t="s">
-        <v>106</v>
+        <v>288</v>
       </c>
       <c r="Z38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA38" s="4" t="s">
-        <v>106</v>
+        <v>288</v>
       </c>
       <c r="AB38" s="4">
         <v>5</v>
@@ -4694,13 +4697,13 @@
         <v>70</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>124</v>
@@ -4730,13 +4733,13 @@
         <v>1</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U39" s="4">
         <v>0</v>
@@ -4745,19 +4748,19 @@
         <v>0</v>
       </c>
       <c r="W39" s="4" t="s">
-        <v>107</v>
+        <v>252</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y39" s="4" t="s">
-        <v>107</v>
+        <v>277</v>
       </c>
       <c r="Z39" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA39" s="4" t="s">
-        <v>107</v>
+        <v>277</v>
       </c>
       <c r="AB39" s="4">
         <v>5</v>
@@ -4777,13 +4780,13 @@
         <v>70</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>71</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>124</v>
@@ -4798,7 +4801,7 @@
         <v>108</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>75</v>
@@ -4813,13 +4816,13 @@
         <v>1</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="U40" s="4">
         <v>0</v>
@@ -4828,19 +4831,19 @@
         <v>0</v>
       </c>
       <c r="W40" s="4" t="s">
-        <v>108</v>
+        <v>251</v>
       </c>
       <c r="X40" s="4" t="s">
         <v>124</v>
       </c>
       <c r="Y40" s="4" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="Z40" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA40" s="4" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="AB40" s="4">
         <v>5</v>
@@ -4854,16 +4857,16 @@
         <v>126</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>241</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>125</v>
@@ -4887,13 +4890,13 @@
         <v>125</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U41" s="4" t="s">
         <v>76</v>
@@ -4902,19 +4905,19 @@
         <v>76</v>
       </c>
       <c r="W41" s="4" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="X41" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="Z41" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA41" s="4" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="AB41" s="4" t="s">
         <v>125</v>
@@ -4931,13 +4934,13 @@
         <v>238</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>241</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>125</v>
@@ -4961,13 +4964,13 @@
         <v>125</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="U42" s="4" t="s">
         <v>76</v>
@@ -4976,19 +4979,19 @@
         <v>76</v>
       </c>
       <c r="W42" s="4" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="X42" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>243</v>
+        <v>288</v>
       </c>
       <c r="Z42" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA42" s="4" t="s">
-        <v>243</v>
+        <v>288</v>
       </c>
       <c r="AB42" s="4" t="s">
         <v>125</v>
@@ -5005,13 +5008,13 @@
         <v>239</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>241</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>125</v>
@@ -5035,13 +5038,13 @@
         <v>125</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="U43" s="4" t="s">
         <v>76</v>
@@ -5050,19 +5053,19 @@
         <v>76</v>
       </c>
       <c r="W43" s="4" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="X43" s="4" t="s">
         <v>125</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>244</v>
+        <v>288</v>
       </c>
       <c r="Z43" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA43" s="4" t="s">
-        <v>244</v>
+        <v>288</v>
       </c>
       <c r="AB43" s="4" t="s">
         <v>125</v>
@@ -5079,13 +5082,13 @@
         <v>240</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>241</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>125</v>
@@ -5094,28 +5097,28 @@
         <v>72</v>
       </c>
       <c r="M44" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="R44" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="P44" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q44" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>124</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="U44" s="4" t="s">
         <v>76</v>
@@ -5124,19 +5127,19 @@
         <v>76</v>
       </c>
       <c r="W44" s="4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="X44" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="Z44" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA44" s="4" t="s">
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="AB44" s="4" t="s">
         <v>125</v>
@@ -5144,31 +5147,31 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>241</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>143</v>
@@ -5186,13 +5189,13 @@
         <v>125</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="S45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="U45" s="4" t="s">
         <v>76</v>
@@ -5201,19 +5204,19 @@
         <v>76</v>
       </c>
       <c r="W45" s="4" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="X45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="Y45" s="4" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="Z45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA45" s="4" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="AB45" s="4" t="s">
         <v>76</v>
@@ -5277,7 +5280,7 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5330,13 +5333,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>68</v>
@@ -5359,10 +5362,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>68</v>
@@ -5385,10 +5388,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>68</v>
@@ -5411,10 +5414,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>68</v>
@@ -5437,10 +5440,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>68</v>
@@ -5463,10 +5466,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>68</v>
@@ -5489,10 +5492,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>68</v>
@@ -5515,10 +5518,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>68</v>
@@ -5541,10 +5544,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>68</v>
@@ -5567,10 +5570,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>68</v>
@@ -5593,10 +5596,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>68</v>
@@ -5616,7 +5619,7 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5679,13 +5682,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>68</v>
@@ -5714,13 +5717,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>68</v>
@@ -5749,13 +5752,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>84</v>
+        <v>259</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>68</v>
@@ -5784,13 +5787,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>85</v>
+        <v>251</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>68</v>
@@ -5819,13 +5822,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>68</v>
@@ -5854,13 +5857,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>87</v>
+        <v>253</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>68</v>
@@ -5889,13 +5892,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>68</v>
@@ -5924,13 +5927,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>68</v>
@@ -5959,13 +5962,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>90</v>
+        <v>250</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>68</v>
@@ -5994,13 +5997,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>91</v>
+        <v>254</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>68</v>
@@ -6029,13 +6032,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>92</v>
+        <v>253</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>68</v>
@@ -6064,13 +6067,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>93</v>
+        <v>251</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>93</v>
+        <v>251</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>93</v>
+        <v>251</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>68</v>
@@ -6099,13 +6102,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>94</v>
+        <v>252</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>94</v>
+        <v>252</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>94</v>
+        <v>252</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>68</v>
@@ -6134,13 +6137,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>68</v>
@@ -6169,13 +6172,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>96</v>
+        <v>251</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>96</v>
+        <v>251</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>96</v>
+        <v>251</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>68</v>
@@ -6204,13 +6207,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>97</v>
+        <v>252</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>68</v>
@@ -6239,13 +6242,13 @@
         <v>0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>98</v>
+        <v>253</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>98</v>
+        <v>253</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>98</v>
+        <v>253</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>68</v>
@@ -6274,13 +6277,13 @@
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>99</v>
+        <v>254</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>99</v>
+        <v>254</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>99</v>
+        <v>254</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>68</v>
@@ -6309,13 +6312,13 @@
         <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>100</v>
+        <v>253</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>68</v>
@@ -6344,13 +6347,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>68</v>
@@ -6379,13 +6382,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>102</v>
+        <v>254</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>68</v>
@@ -6414,13 +6417,13 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>68</v>
@@ -6449,13 +6452,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>68</v>
@@ -6467,10 +6470,10 @@
         <v>76</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.15">
@@ -6484,13 +6487,13 @@
         <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>103</v>
+        <v>252</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>103</v>
+        <v>252</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>68</v>
@@ -6502,10 +6505,10 @@
         <v>76</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.15">
@@ -6513,19 +6516,19 @@
         <v>240</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>239</v>
@@ -6537,10 +6540,10 @@
         <v>76</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.15">
@@ -6554,13 +6557,13 @@
         <v>76</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>103</v>
+        <v>254</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>103</v>
+        <v>254</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>103</v>
+        <v>254</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>239</v>
@@ -6572,10 +6575,10 @@
         <v>76</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -6588,8 +6591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="302" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6625,10 +6628,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>169</v>
+        <v>253</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -6702,7 +6705,7 @@
         <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
@@ -6713,7 +6716,7 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
@@ -6724,7 +6727,7 @@
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -6841,13 +6844,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.15">
@@ -6855,19 +6858,19 @@
         <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F6">
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -6881,7 +6884,7 @@
   <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="262" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E3" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6915,7 +6918,7 @@
         <v>146</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>169</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.15">
@@ -6929,7 +6932,7 @@
         <v>146</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>83</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.15">
@@ -6943,7 +6946,7 @@
         <v>146</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.15">
@@ -6957,7 +6960,7 @@
         <v>148</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>85</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
@@ -6971,7 +6974,7 @@
         <v>148</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>86</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
@@ -6985,12 +6988,13 @@
         <v>150</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>87</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6999,7 +7003,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J3" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7071,7 +7075,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>169</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -7100,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>82</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -7183,7 +7187,7 @@
         <v>53</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -7274,7 +7278,7 @@
         <v>188</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -7370,7 +7374,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -7409,7 +7413,7 @@
         <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
@@ -7417,7 +7421,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
         <v>239</v>
@@ -7438,16 +7442,16 @@
         <v>2</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -7456,7 +7460,7 @@
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -7470,7 +7474,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7527,7 +7531,7 @@
         <v>100</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -7550,7 +7554,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>82</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -7564,7 +7568,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="304" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7609,7 +7613,7 @@
         <v>207</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>305</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
#1 fix unit-test & explore file system
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE4547D-60E3-42B6-B63C-30CA580B6737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B0590-DA38-4504-B27B-58394385A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -946,10 +946,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>.\files\test\admin_c_1651157940.0784883\SampleTestPaper_admin_ex_1651157940.0784883.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2020-12-12 00:00:00</t>
   </si>
   <si>
@@ -957,18 +953,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>.\files\test\admin_c_1651198092.9064405\SampleTest2_admin_ex_1651198092.9064405.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>样例3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>.\files\test\test_content_exam_1\sample3.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1077,6 +1065,18 @@
   </si>
   <si>
     <t>2022-5-4 00:00:06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./files/test/admin_c_1651157940.0784883/SampleTestPaper_admin_ex_1651157940.0784883.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./files/test/admin_c_1651198092.9064405/SampleTest2_admin_ex_1651198092.9064405.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>./files/test/test_content_exam_1/sample3.csv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1494,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="T10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="W27" sqref="W27:W35"/>
     </sheetView>
   </sheetViews>
@@ -1626,7 +1626,7 @@
         <v>70</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>71</v>
@@ -1668,7 +1668,7 @@
         <v>75</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="U2" s="4">
         <v>0</v>
@@ -1683,13 +1683,13 @@
         <v>125</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="Z2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AB2" s="4">
         <v>5</v>
@@ -1709,7 +1709,7 @@
         <v>70</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>71</v>
@@ -1751,7 +1751,7 @@
         <v>125</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="U3" s="4">
         <v>0</v>
@@ -1766,13 +1766,13 @@
         <v>125</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Z3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AB3" s="4">
         <v>5</v>
@@ -1792,7 +1792,7 @@
         <v>70</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>71</v>
@@ -1834,7 +1834,7 @@
         <v>125</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="U4" s="4">
         <v>0</v>
@@ -1849,13 +1849,13 @@
         <v>1</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="Z4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AB4" s="4">
         <v>5</v>
@@ -1875,7 +1875,7 @@
         <v>70</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>71</v>
@@ -1917,7 +1917,7 @@
         <v>125</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="U5" s="4">
         <v>0</v>
@@ -1932,13 +1932,13 @@
         <v>125</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="Z5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="AB5" s="4">
         <v>5</v>
@@ -1958,7 +1958,7 @@
         <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>71</v>
@@ -2000,7 +2000,7 @@
         <v>76</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="U6" s="4">
         <v>0</v>
@@ -2015,13 +2015,13 @@
         <v>125</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Z6" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AB6" s="4">
         <v>5</v>
@@ -2041,7 +2041,7 @@
         <v>70</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>71</v>
@@ -2083,7 +2083,7 @@
         <v>125</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="U7" s="4">
         <v>0</v>
@@ -2098,13 +2098,13 @@
         <v>125</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Z7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="AB7" s="4">
         <v>5</v>
@@ -2124,7 +2124,7 @@
         <v>70</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>71</v>
@@ -2166,7 +2166,7 @@
         <v>124</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="U8" s="4">
         <v>0</v>
@@ -2181,13 +2181,13 @@
         <v>125</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB8" s="4">
         <v>5</v>
@@ -2207,7 +2207,7 @@
         <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>71</v>
@@ -2249,7 +2249,7 @@
         <v>76</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="U9" s="4">
         <v>0</v>
@@ -2264,13 +2264,13 @@
         <v>125</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="Z9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="AB9" s="4">
         <v>5</v>
@@ -2290,7 +2290,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>71</v>
@@ -2332,7 +2332,7 @@
         <v>124</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="U10" s="4">
         <v>0</v>
@@ -2347,13 +2347,13 @@
         <v>125</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="Z10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="AB10" s="4">
         <v>5</v>
@@ -2373,7 +2373,7 @@
         <v>70</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>71</v>
@@ -2415,7 +2415,7 @@
         <v>124</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="U11" s="4">
         <v>0</v>
@@ -2430,13 +2430,13 @@
         <v>125</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="Z11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="AB11" s="4">
         <v>5</v>
@@ -2456,7 +2456,7 @@
         <v>70</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>71</v>
@@ -2498,7 +2498,7 @@
         <v>124</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="U12" s="4">
         <v>0</v>
@@ -2513,13 +2513,13 @@
         <v>125</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="Z12" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA12" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="AB12" s="4">
         <v>5</v>
@@ -2539,7 +2539,7 @@
         <v>70</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>71</v>
@@ -2581,7 +2581,7 @@
         <v>124</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="U13" s="4">
         <v>0</v>
@@ -2596,13 +2596,13 @@
         <v>125</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="Z13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="AB13" s="4">
         <v>5</v>
@@ -2622,7 +2622,7 @@
         <v>70</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>71</v>
@@ -2664,7 +2664,7 @@
         <v>143</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="U14" s="4">
         <v>0</v>
@@ -2679,13 +2679,13 @@
         <v>125</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="Z14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="AB14" s="4">
         <v>5</v>
@@ -2705,7 +2705,7 @@
         <v>70</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>71</v>
@@ -2747,7 +2747,7 @@
         <v>143</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="U15" s="4">
         <v>0</v>
@@ -2762,13 +2762,13 @@
         <v>125</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="Z15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AB15" s="4">
         <v>5</v>
@@ -2788,7 +2788,7 @@
         <v>70</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>71</v>
@@ -2830,7 +2830,7 @@
         <v>143</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="U16" s="4">
         <v>0</v>
@@ -2845,13 +2845,13 @@
         <v>125</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="Z16" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AB16" s="4">
         <v>5</v>
@@ -2871,7 +2871,7 @@
         <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>71</v>
@@ -2913,7 +2913,7 @@
         <v>125</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="U17" s="4">
         <v>0</v>
@@ -2928,13 +2928,13 @@
         <v>125</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="Z17" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="AB17" s="4">
         <v>5</v>
@@ -2954,7 +2954,7 @@
         <v>70</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>137</v>
@@ -2996,7 +2996,7 @@
         <v>75</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="U18" s="4">
         <v>0</v>
@@ -3011,13 +3011,13 @@
         <v>125</v>
       </c>
       <c r="Y18" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="Z18" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="AB18" s="4">
         <v>5</v>
@@ -3037,7 +3037,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>138</v>
@@ -3079,7 +3079,7 @@
         <v>124</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U19" s="4">
         <v>0</v>
@@ -3094,13 +3094,13 @@
         <v>76</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z19" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB19" s="4" t="s">
         <v>144</v>
@@ -3120,7 +3120,7 @@
         <v>70</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>139</v>
@@ -3162,7 +3162,7 @@
         <v>143</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U20" s="4">
         <v>0</v>
@@ -3177,13 +3177,13 @@
         <v>125</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB20" s="4" t="s">
         <v>144</v>
@@ -3203,7 +3203,7 @@
         <v>70</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>140</v>
@@ -3245,7 +3245,7 @@
         <v>143</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U21" s="4">
         <v>0</v>
@@ -3260,13 +3260,13 @@
         <v>143</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA21" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB21" s="4" t="s">
         <v>144</v>
@@ -3286,7 +3286,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>139</v>
@@ -3328,7 +3328,7 @@
         <v>244</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="U22" s="4">
         <v>0</v>
@@ -3343,13 +3343,13 @@
         <v>125</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="Z22" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AB22" s="4" t="s">
         <v>144</v>
@@ -3369,7 +3369,7 @@
         <v>70</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>157</v>
@@ -3411,7 +3411,7 @@
         <v>244</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U23" s="4">
         <v>0</v>
@@ -3426,13 +3426,13 @@
         <v>76</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z23" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB23" s="4">
         <v>5</v>
@@ -3452,7 +3452,7 @@
         <v>70</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>157</v>
@@ -3494,7 +3494,7 @@
         <v>244</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U24" s="4">
         <v>0</v>
@@ -3509,13 +3509,13 @@
         <v>76</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z24" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB24" s="4">
         <v>5</v>
@@ -3535,7 +3535,7 @@
         <v>70</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>157</v>
@@ -3577,7 +3577,7 @@
         <v>244</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U25" s="4">
         <v>0</v>
@@ -3592,13 +3592,13 @@
         <v>75</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z25" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA25" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB25" s="4">
         <v>5</v>
@@ -3618,7 +3618,7 @@
         <v>70</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>158</v>
@@ -3660,7 +3660,7 @@
         <v>244</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U26" s="4">
         <v>0</v>
@@ -3675,13 +3675,13 @@
         <v>75</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z26" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB26" s="4">
         <v>5</v>
@@ -3701,7 +3701,7 @@
         <v>70</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>158</v>
@@ -3743,7 +3743,7 @@
         <v>244</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U27" s="4">
         <v>0</v>
@@ -3758,13 +3758,13 @@
         <v>75</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z27" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB27" s="4">
         <v>5</v>
@@ -3784,7 +3784,7 @@
         <v>70</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>158</v>
@@ -3826,7 +3826,7 @@
         <v>244</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U28" s="4">
         <v>0</v>
@@ -3841,13 +3841,13 @@
         <v>75</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z28" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB28" s="4">
         <v>5</v>
@@ -3867,7 +3867,7 @@
         <v>70</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>71</v>
@@ -3909,7 +3909,7 @@
         <v>244</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U29" s="4">
         <v>0</v>
@@ -3924,13 +3924,13 @@
         <v>124</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z29" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB29" s="4">
         <v>5</v>
@@ -3950,7 +3950,7 @@
         <v>70</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>71</v>
@@ -3992,7 +3992,7 @@
         <v>244</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="U30" s="4">
         <v>0</v>
@@ -4007,13 +4007,13 @@
         <v>124</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="Z30" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA30" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AB30" s="4">
         <v>5</v>
@@ -4033,7 +4033,7 @@
         <v>70</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>71</v>
@@ -4075,7 +4075,7 @@
         <v>124</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U31" s="4">
         <v>0</v>
@@ -4090,13 +4090,13 @@
         <v>124</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z31" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA31" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB31" s="4">
         <v>5</v>
@@ -4116,7 +4116,7 @@
         <v>70</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>71</v>
@@ -4158,7 +4158,7 @@
         <v>124</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U32" s="4">
         <v>0</v>
@@ -4173,13 +4173,13 @@
         <v>124</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z32" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA32" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB32" s="4">
         <v>5</v>
@@ -4199,7 +4199,7 @@
         <v>70</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>71</v>
@@ -4241,7 +4241,7 @@
         <v>76</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U33" s="4">
         <v>0</v>
@@ -4256,13 +4256,13 @@
         <v>124</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA33" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB33" s="4">
         <v>5</v>
@@ -4282,7 +4282,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>71</v>
@@ -4324,7 +4324,7 @@
         <v>125</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U34" s="4">
         <v>0</v>
@@ -4339,13 +4339,13 @@
         <v>124</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z34" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA34" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB34" s="4">
         <v>5</v>
@@ -4365,7 +4365,7 @@
         <v>70</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>71</v>
@@ -4407,7 +4407,7 @@
         <v>143</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U35" s="4">
         <v>0</v>
@@ -4422,13 +4422,13 @@
         <v>124</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z35" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB35" s="4">
         <v>5</v>
@@ -4448,7 +4448,7 @@
         <v>70</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>71</v>
@@ -4490,7 +4490,7 @@
         <v>143</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="U36" s="4">
         <v>0</v>
@@ -4505,13 +4505,13 @@
         <v>124</v>
       </c>
       <c r="Y36" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Z36" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA36" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AB36" s="4">
         <v>5</v>
@@ -4531,7 +4531,7 @@
         <v>70</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>71</v>
@@ -4573,7 +4573,7 @@
         <v>244</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="U37" s="4">
         <v>0</v>
@@ -4588,13 +4588,13 @@
         <v>124</v>
       </c>
       <c r="Y37" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Z37" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA37" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="AB37" s="4">
         <v>5</v>
@@ -4614,7 +4614,7 @@
         <v>70</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>71</v>
@@ -4656,7 +4656,7 @@
         <v>244</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="U38" s="4">
         <v>0</v>
@@ -4671,13 +4671,13 @@
         <v>124</v>
       </c>
       <c r="Y38" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z38" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA38" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB38" s="4">
         <v>5</v>
@@ -4697,7 +4697,7 @@
         <v>70</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>71</v>
@@ -4739,7 +4739,7 @@
         <v>124</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U39" s="4">
         <v>0</v>
@@ -4754,13 +4754,13 @@
         <v>124</v>
       </c>
       <c r="Y39" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z39" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA39" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB39" s="4">
         <v>5</v>
@@ -4780,7 +4780,7 @@
         <v>70</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>71</v>
@@ -4822,7 +4822,7 @@
         <v>124</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="U40" s="4">
         <v>0</v>
@@ -4837,13 +4837,13 @@
         <v>124</v>
       </c>
       <c r="Y40" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z40" s="4" t="b">
         <v>1</v>
       </c>
       <c r="AA40" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB40" s="4">
         <v>5</v>
@@ -4860,7 +4860,7 @@
         <v>242</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>241</v>
@@ -4896,7 +4896,7 @@
         <v>124</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U41" s="4" t="s">
         <v>76</v>
@@ -4911,13 +4911,13 @@
         <v>125</v>
       </c>
       <c r="Y41" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="Z41" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA41" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AB41" s="4" t="s">
         <v>125</v>
@@ -4934,7 +4934,7 @@
         <v>238</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>241</v>
@@ -4970,7 +4970,7 @@
         <v>124</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="U42" s="4" t="s">
         <v>76</v>
@@ -4985,13 +4985,13 @@
         <v>125</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z42" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA42" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB42" s="4" t="s">
         <v>125</v>
@@ -5008,7 +5008,7 @@
         <v>239</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>241</v>
@@ -5044,7 +5044,7 @@
         <v>124</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="U43" s="4" t="s">
         <v>76</v>
@@ -5059,13 +5059,13 @@
         <v>125</v>
       </c>
       <c r="Y43" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="Z43" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA43" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AB43" s="4" t="s">
         <v>125</v>
@@ -5082,7 +5082,7 @@
         <v>240</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>241</v>
@@ -5118,7 +5118,7 @@
         <v>124</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="U44" s="4" t="s">
         <v>76</v>
@@ -5133,13 +5133,13 @@
         <v>76</v>
       </c>
       <c r="Y44" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="Z44" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA44" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="AB44" s="4" t="s">
         <v>125</v>
@@ -5159,7 +5159,7 @@
         <v>258</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>241</v>
@@ -5195,7 +5195,7 @@
         <v>76</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="U45" s="4" t="s">
         <v>76</v>
@@ -5210,13 +5210,13 @@
         <v>76</v>
       </c>
       <c r="Y45" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="Z45" s="4" t="s">
         <v>76</v>
       </c>
       <c r="AA45" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="AB45" s="4" t="s">
         <v>76</v>
@@ -6516,7 +6516,7 @@
         <v>240</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>76</v>
@@ -6540,7 +6540,7 @@
         <v>76</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>265</v>
@@ -6575,10 +6575,10 @@
         <v>76</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -6918,7 +6918,7 @@
         <v>146</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.15">
@@ -6932,7 +6932,7 @@
         <v>146</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.15">
@@ -6946,7 +6946,7 @@
         <v>146</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.15">
@@ -6960,7 +6960,7 @@
         <v>148</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
@@ -6974,7 +6974,7 @@
         <v>148</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.15">
@@ -6988,7 +6988,7 @@
         <v>150</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -7075,7 +7075,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -7104,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -7118,7 +7118,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7278,7 +7278,7 @@
         <v>188</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>268</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -7374,7 +7374,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -7413,7 +7413,7 @@
         <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>271</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
@@ -7421,7 +7421,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C7" t="s">
         <v>239</v>
@@ -7442,16 +7442,16 @@
         <v>2</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -7460,7 +7460,7 @@
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -7474,7 +7474,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7531,7 +7531,7 @@
         <v>100</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
@@ -7554,7 +7554,7 @@
         <v>100</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -7613,7 +7613,7 @@
         <v>207</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>208</v>

</xml_diff>

<commit_message>
#39 #40 api for recode and comits done, writing testcase
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B0590-DA38-4504-B27B-58394385A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F25849-0999-2A45-A729-656BAF9584DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="309">
   <si>
     <t>username</t>
   </si>
@@ -1077,6 +1077,17 @@
   </si>
   <si>
     <t>./files/test/test_content_exam_1/sample3.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:12</t>
+  </si>
+  <si>
+    <t>今天不错</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1084,7 +1095,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1494,39 +1505,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView topLeftCell="T10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27:W35"/>
+    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="4"/>
+    <col min="9" max="9" width="8.83203125" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="4"/>
-    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.875" style="4"/>
+    <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.83203125" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1612,7 +1623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -1695,7 +1706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>110</v>
       </c>
@@ -1861,7 +1872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>111</v>
       </c>
@@ -1944,7 +1955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
         <v>112</v>
       </c>
@@ -2027,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
@@ -2110,7 +2121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
         <v>114</v>
       </c>
@@ -2193,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
         <v>115</v>
       </c>
@@ -2276,7 +2287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
         <v>116</v>
       </c>
@@ -2359,7 +2370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
         <v>117</v>
       </c>
@@ -2442,7 +2453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28">
       <c r="A12" s="4" t="s">
         <v>118</v>
       </c>
@@ -2525,7 +2536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28">
       <c r="A13" s="4" t="s">
         <v>119</v>
       </c>
@@ -2608,7 +2619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28">
       <c r="A14" s="4" t="s">
         <v>120</v>
       </c>
@@ -2691,7 +2702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28">
       <c r="A15" s="4" t="s">
         <v>121</v>
       </c>
@@ -2774,7 +2785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28">
       <c r="A16" s="4" t="s">
         <v>122</v>
       </c>
@@ -2857,7 +2868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -2940,7 +2951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28">
       <c r="A18" s="4" t="s">
         <v>128</v>
       </c>
@@ -3023,7 +3034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28">
       <c r="A19" s="4" t="s">
         <v>130</v>
       </c>
@@ -3106,7 +3117,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28">
       <c r="A20" s="4" t="s">
         <v>132</v>
       </c>
@@ -3189,7 +3200,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28">
       <c r="A21" s="4" t="s">
         <v>134</v>
       </c>
@@ -3272,7 +3283,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28">
       <c r="A22" s="4" t="s">
         <v>136</v>
       </c>
@@ -3355,7 +3366,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28">
       <c r="A23" s="4" t="s">
         <v>146</v>
       </c>
@@ -3438,7 +3449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28">
       <c r="A24" s="4" t="s">
         <v>148</v>
       </c>
@@ -3521,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28">
       <c r="A25" s="4" t="s">
         <v>150</v>
       </c>
@@ -3604,7 +3615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28">
       <c r="A26" s="4" t="s">
         <v>152</v>
       </c>
@@ -3687,7 +3698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -3770,7 +3781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28">
       <c r="A29" s="4" t="s">
         <v>195</v>
       </c>
@@ -3936,7 +3947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28">
       <c r="A30" s="4" t="s">
         <v>196</v>
       </c>
@@ -4019,7 +4030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28">
       <c r="A31" s="4" t="s">
         <v>197</v>
       </c>
@@ -4102,7 +4113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28">
       <c r="A32" s="4" t="s">
         <v>198</v>
       </c>
@@ -4185,7 +4196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28">
       <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
@@ -4268,7 +4279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28">
       <c r="A34" s="4" t="s">
         <v>200</v>
       </c>
@@ -4351,7 +4362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28">
       <c r="A35" s="4" t="s">
         <v>201</v>
       </c>
@@ -4434,7 +4445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28">
       <c r="A36" s="4" t="s">
         <v>202</v>
       </c>
@@ -4517,7 +4528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28">
       <c r="A37" s="4" t="s">
         <v>203</v>
       </c>
@@ -4600,7 +4611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28">
       <c r="A38" s="4" t="s">
         <v>204</v>
       </c>
@@ -4683,7 +4694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28">
       <c r="A39" s="4" t="s">
         <v>205</v>
       </c>
@@ -4766,7 +4777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28">
       <c r="A40" s="4" t="s">
         <v>206</v>
       </c>
@@ -4849,7 +4860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4923,7 +4934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28">
       <c r="A42" s="4" t="s">
         <v>238</v>
       </c>
@@ -4997,7 +5008,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28">
       <c r="A43" s="4" t="s">
         <v>239</v>
       </c>
@@ -5071,7 +5082,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28">
       <c r="A44" s="4" t="s">
         <v>240</v>
       </c>
@@ -5145,7 +5156,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28">
       <c r="A45" s="4" t="s">
         <v>257</v>
       </c>
@@ -5283,14 +5294,14 @@
       <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5319,7 +5330,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5348,7 +5359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5374,7 +5385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5400,7 +5411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5426,7 +5437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5452,7 +5463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5478,7 +5489,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5504,7 +5515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -5530,7 +5541,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -5556,7 +5567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -5582,7 +5593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -5622,21 +5633,21 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
-    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5671,7 +5682,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5706,7 +5717,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5741,7 +5752,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5776,7 +5787,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5811,7 +5822,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5846,7 +5857,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5881,7 +5892,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5916,7 +5927,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -5951,7 +5962,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -5986,7 +5997,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -6021,7 +6032,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -6056,7 +6067,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12">
       <c r="B13" s="7" t="s">
         <v>127</v>
       </c>
@@ -6091,7 +6102,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12">
       <c r="B14" s="7" t="s">
         <v>129</v>
       </c>
@@ -6126,7 +6137,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12">
       <c r="B15" s="7" t="s">
         <v>131</v>
       </c>
@@ -6161,7 +6172,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12">
       <c r="B16" s="7" t="s">
         <v>133</v>
       </c>
@@ -6196,7 +6207,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:12">
       <c r="B17" s="7" t="s">
         <v>135</v>
       </c>
@@ -6231,7 +6242,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:12">
       <c r="B18" s="7" t="s">
         <v>145</v>
       </c>
@@ -6266,7 +6277,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:12">
       <c r="B19" s="7" t="s">
         <v>147</v>
       </c>
@@ -6301,7 +6312,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12">
       <c r="B20" s="7" t="s">
         <v>149</v>
       </c>
@@ -6336,7 +6347,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:12">
       <c r="B21" s="7" t="s">
         <v>151</v>
       </c>
@@ -6371,7 +6382,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:12">
       <c r="B22" s="7" t="s">
         <v>153</v>
       </c>
@@ -6406,7 +6417,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12">
       <c r="B23" s="7" t="s">
         <v>155</v>
       </c>
@@ -6441,7 +6452,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:12">
       <c r="B24" s="4" t="s">
         <v>239</v>
       </c>
@@ -6476,7 +6487,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:12">
       <c r="B25" s="4" t="s">
         <v>240</v>
       </c>
@@ -6511,7 +6522,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:12">
       <c r="B26" s="4" t="s">
         <v>240</v>
       </c>
@@ -6546,7 +6557,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:12">
       <c r="B27" s="4" t="s">
         <v>240</v>
       </c>
@@ -6591,16 +6602,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
+    <sheetView zoomScale="302" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6617,7 +6628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -6648,9 +6659,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6664,7 +6675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6675,7 +6686,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6686,7 +6697,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4">
         <v>2</v>
       </c>
@@ -6697,7 +6708,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5">
         <v>0</v>
       </c>
@@ -6708,7 +6719,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6719,7 +6730,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7">
         <v>2</v>
       </c>
@@ -6738,22 +6749,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:G6"/>
+  <dimension ref="B1:G7"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6773,7 +6784,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -6793,7 +6804,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>129</v>
       </c>
@@ -6813,7 +6824,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>131</v>
       </c>
@@ -6833,7 +6844,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>239</v>
       </c>
@@ -6853,7 +6864,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7">
       <c r="B6" t="s">
         <v>239</v>
       </c>
@@ -6871,6 +6882,26 @@
       </c>
       <c r="G6" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -6881,19 +6912,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="262" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E3"/>
+    <sheetView tabSelected="1" zoomScale="262" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -6907,7 +6938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>170</v>
       </c>
@@ -6921,7 +6952,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>171</v>
       </c>
@@ -6935,7 +6966,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>172</v>
       </c>
@@ -6949,7 +6980,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>173</v>
       </c>
@@ -6963,7 +6994,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>174</v>
       </c>
@@ -6977,7 +7008,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>175</v>
       </c>
@@ -6989,6 +7020,20 @@
       </c>
       <c r="E7" s="4" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -7006,18 +7051,18 @@
       <selection activeCell="J3" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="4" width="8.875" style="4"/>
+    <col min="1" max="4" width="8.83203125" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="4"/>
-    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>182</v>
       </c>
@@ -7049,7 +7094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7078,7 +7123,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7117,21 +7162,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="4"/>
+    <col min="14" max="15" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7190,7 +7235,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7234,7 +7279,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7281,7 +7326,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7325,7 +7370,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7369,7 +7414,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7416,7 +7461,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7477,15 +7522,15 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7511,7 +7556,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7534,7 +7579,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7571,12 +7616,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7599,7 +7644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7636,12 +7681,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -7652,7 +7697,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
         <v>125</v>
       </c>
@@ -7663,7 +7708,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
         <v>125</v>
       </c>
@@ -7674,7 +7719,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="B4" s="4" t="s">
         <v>143</v>
       </c>
@@ -7685,7 +7730,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4">
       <c r="B5" s="4" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
#39 testcases for commits and socres added
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F25849-0999-2A45-A729-656BAF9584DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AF377-DDA7-D544-B127-1DE895F781E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -6914,7 +6914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="262" workbookViewId="0">
+    <sheetView zoomScale="262" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix cover bug, remove cover
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2F6EE-14E3-4FE9-A4D0-525AC540C82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672497E2-ADFC-4CA8-BDA3-E783870BFE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="2880" windowWidth="30735" windowHeight="15150" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="3210" windowWidth="30735" windowHeight="15150" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -7162,7 +7162,7 @@
         <v>292</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#32 add teacher_newcomer_list_by_name api fix some tiny bug
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AF377-DDA7-D544-B127-1DE895F781E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC1FFE2-3301-1043-8C67-E70DC9CAEFC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="309">
   <si>
     <t>username</t>
   </si>
@@ -1505,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="R10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1696,8 +1696,8 @@
       <c r="Y2" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="Z2" s="4" t="b">
-        <v>1</v>
+      <c r="Z2" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>289</v>
@@ -1759,7 +1759,7 @@
         <v>251</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="T3" s="4" t="s">
         <v>290</v>
@@ -1779,8 +1779,8 @@
       <c r="Y3" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="Z3" s="4" t="b">
-        <v>1</v>
+      <c r="Z3" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA3" s="4" t="s">
         <v>290</v>
@@ -1862,8 +1862,8 @@
       <c r="Y4" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="Z4" s="4" t="b">
-        <v>1</v>
+      <c r="Z4" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA4" s="4" t="s">
         <v>291</v>
@@ -1945,8 +1945,8 @@
       <c r="Y5" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="Z5" s="4" t="b">
-        <v>1</v>
+      <c r="Z5" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA5" s="4" t="s">
         <v>292</v>
@@ -2028,8 +2028,8 @@
       <c r="Y6" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="Z6" s="4" t="b">
-        <v>1</v>
+      <c r="Z6" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA6" s="4" t="s">
         <v>283</v>
@@ -2111,8 +2111,8 @@
       <c r="Y7" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="Z7" s="4" t="b">
-        <v>1</v>
+      <c r="Z7" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA7" s="4" t="s">
         <v>284</v>
@@ -2194,8 +2194,8 @@
       <c r="Y8" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Z8" s="4" t="b">
-        <v>1</v>
+      <c r="Z8" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA8" s="4" t="s">
         <v>285</v>
@@ -2277,8 +2277,8 @@
       <c r="Y9" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="Z9" s="4" t="b">
-        <v>1</v>
+      <c r="Z9" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA9" s="4" t="s">
         <v>275</v>
@@ -2360,8 +2360,8 @@
       <c r="Y10" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="Z10" s="4" t="b">
-        <v>1</v>
+      <c r="Z10" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA10" s="4" t="s">
         <v>276</v>
@@ -2443,8 +2443,8 @@
       <c r="Y11" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="Z11" s="4" t="b">
-        <v>1</v>
+      <c r="Z11" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA11" s="4" t="s">
         <v>277</v>
@@ -2526,8 +2526,8 @@
       <c r="Y12" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="Z12" s="4" t="b">
-        <v>1</v>
+      <c r="Z12" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA12" s="4" t="s">
         <v>278</v>
@@ -2609,8 +2609,8 @@
       <c r="Y13" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="Z13" s="4" t="b">
-        <v>1</v>
+      <c r="Z13" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA13" s="4" t="s">
         <v>279</v>
@@ -2692,8 +2692,8 @@
       <c r="Y14" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="Z14" s="4" t="b">
-        <v>1</v>
+      <c r="Z14" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA14" s="4" t="s">
         <v>280</v>
@@ -2775,8 +2775,8 @@
       <c r="Y15" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="Z15" s="4" t="b">
-        <v>1</v>
+      <c r="Z15" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA15" s="4" t="s">
         <v>281</v>
@@ -2858,8 +2858,8 @@
       <c r="Y16" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="Z16" s="4" t="b">
-        <v>1</v>
+      <c r="Z16" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA16" s="4" t="s">
         <v>282</v>
@@ -2941,8 +2941,8 @@
       <c r="Y17" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="Z17" s="4" t="b">
-        <v>1</v>
+      <c r="Z17" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA17" s="4" t="s">
         <v>293</v>
@@ -3024,8 +3024,8 @@
       <c r="Y18" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="Z18" s="4" t="b">
-        <v>1</v>
+      <c r="Z18" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA18" s="4" t="s">
         <v>286</v>
@@ -3937,8 +3937,8 @@
       <c r="Y29" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z29" s="4" t="b">
-        <v>1</v>
+      <c r="Z29" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA29" s="4" t="s">
         <v>274</v>
@@ -4020,8 +4020,8 @@
       <c r="Y30" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="Z30" s="4" t="b">
-        <v>1</v>
+      <c r="Z30" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA30" s="4" t="s">
         <v>288</v>
@@ -4103,8 +4103,8 @@
       <c r="Y31" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z31" s="4" t="b">
-        <v>1</v>
+      <c r="Z31" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA31" s="4" t="s">
         <v>274</v>
@@ -4186,8 +4186,8 @@
       <c r="Y32" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z32" s="4" t="b">
-        <v>1</v>
+      <c r="Z32" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA32" s="4" t="s">
         <v>274</v>
@@ -4269,8 +4269,8 @@
       <c r="Y33" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z33" s="4" t="b">
-        <v>1</v>
+      <c r="Z33" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA33" s="4" t="s">
         <v>274</v>
@@ -4352,8 +4352,8 @@
       <c r="Y34" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z34" s="4" t="b">
-        <v>1</v>
+      <c r="Z34" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA34" s="4" t="s">
         <v>274</v>
@@ -4435,8 +4435,8 @@
       <c r="Y35" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z35" s="4" t="b">
-        <v>1</v>
+      <c r="Z35" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA35" s="4" t="s">
         <v>274</v>
@@ -4518,8 +4518,8 @@
       <c r="Y36" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="Z36" s="4" t="b">
-        <v>1</v>
+      <c r="Z36" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA36" s="4" t="s">
         <v>283</v>
@@ -4601,8 +4601,8 @@
       <c r="Y37" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="Z37" s="4" t="b">
-        <v>1</v>
+      <c r="Z37" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA37" s="4" t="s">
         <v>284</v>
@@ -4684,8 +4684,8 @@
       <c r="Y38" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Z38" s="4" t="b">
-        <v>1</v>
+      <c r="Z38" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA38" s="4" t="s">
         <v>285</v>
@@ -4767,8 +4767,8 @@
       <c r="Y39" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="Z39" s="4" t="b">
-        <v>1</v>
+      <c r="Z39" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA39" s="4" t="s">
         <v>274</v>
@@ -4850,8 +4850,8 @@
       <c r="Y40" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Z40" s="4" t="b">
-        <v>1</v>
+      <c r="Z40" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="AA40" s="4" t="s">
         <v>285</v>
@@ -5073,7 +5073,7 @@
         <v>285</v>
       </c>
       <c r="Z43" s="4" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="AA43" s="4" t="s">
         <v>285</v>

</xml_diff>

<commit_message>
#43 Fixed API for task file
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7918FA-5537-354F-B8DA-41A75A3A54D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AC7BAD-95CC-49A4-8A9D-6F8FBEEEC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="3220" windowWidth="30740" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="317">
   <si>
     <t>username</t>
   </si>
@@ -1092,6 +1092,34 @@
   </si>
   <si>
     <t>isTemplate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fileTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taskFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.\files\task\admin_c_1651829254.4129157\6磁场-21_admin_tsk_1651244631_admin_tsk_1651829254.4139159.pdf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1099,7 +1127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1509,39 +1537,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="G31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="8.875" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.83203125" style="4"/>
-    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.83203125" style="4"/>
+    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.875" style="4"/>
+    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1627,7 +1655,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -1710,7 +1738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
@@ -1793,7 +1821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>110</v>
       </c>
@@ -1876,7 +1904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>111</v>
       </c>
@@ -1959,7 +1987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>112</v>
       </c>
@@ -2042,7 +2070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
@@ -2125,7 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>114</v>
       </c>
@@ -2208,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>115</v>
       </c>
@@ -2291,7 +2319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>116</v>
       </c>
@@ -2374,7 +2402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>117</v>
       </c>
@@ -2457,7 +2485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>118</v>
       </c>
@@ -2540,7 +2568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>119</v>
       </c>
@@ -2623,7 +2651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>120</v>
       </c>
@@ -2706,7 +2734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>121</v>
       </c>
@@ -2789,7 +2817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>122</v>
       </c>
@@ -2872,7 +2900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -2955,7 +2983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>128</v>
       </c>
@@ -3038,7 +3066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>130</v>
       </c>
@@ -3121,7 +3149,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>132</v>
       </c>
@@ -3204,7 +3232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>134</v>
       </c>
@@ -3287,7 +3315,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>136</v>
       </c>
@@ -3370,7 +3398,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>146</v>
       </c>
@@ -3453,7 +3481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>148</v>
       </c>
@@ -3536,7 +3564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>150</v>
       </c>
@@ -3619,7 +3647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>152</v>
       </c>
@@ -3702,7 +3730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -3785,7 +3813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -3868,7 +3896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>195</v>
       </c>
@@ -3951,7 +3979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>196</v>
       </c>
@@ -4034,7 +4062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>197</v>
       </c>
@@ -4117,7 +4145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>198</v>
       </c>
@@ -4200,7 +4228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
@@ -4283,7 +4311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>200</v>
       </c>
@@ -4366,7 +4394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>201</v>
       </c>
@@ -4449,7 +4477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>202</v>
       </c>
@@ -4532,7 +4560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>203</v>
       </c>
@@ -4615,7 +4643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>204</v>
       </c>
@@ -4698,7 +4726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>205</v>
       </c>
@@ -4781,7 +4809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>206</v>
       </c>
@@ -4864,7 +4892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4938,7 +4966,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>238</v>
       </c>
@@ -5012,7 +5040,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>239</v>
       </c>
@@ -5086,7 +5114,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>240</v>
       </c>
@@ -5160,7 +5188,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>257</v>
       </c>
@@ -5298,14 +5326,14 @@
       <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1">
+    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5334,7 +5362,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5363,7 +5391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5389,7 +5417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5415,7 +5443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5441,7 +5469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5467,7 +5495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5493,7 +5521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5519,7 +5547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -5545,7 +5573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -5571,7 +5599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -5597,7 +5625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -5631,27 +5659,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L27"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
-    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4"/>
-    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.875" style="4"/>
+    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1">
+    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5686,7 +5714,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5721,7 +5749,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5756,7 +5784,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5791,7 +5819,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5826,7 +5854,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5861,7 +5889,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5896,7 +5924,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5931,7 +5959,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -5966,7 +5994,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -6001,7 +6029,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -6036,7 +6064,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -6071,7 +6099,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B13" s="7" t="s">
         <v>127</v>
       </c>
@@ -6106,7 +6134,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B14" s="7" t="s">
         <v>129</v>
       </c>
@@ -6141,7 +6169,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B15" s="7" t="s">
         <v>131</v>
       </c>
@@ -6176,7 +6204,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B16" s="7" t="s">
         <v>133</v>
       </c>
@@ -6211,7 +6239,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B17" s="7" t="s">
         <v>135</v>
       </c>
@@ -6246,7 +6274,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B18" s="7" t="s">
         <v>145</v>
       </c>
@@ -6281,7 +6309,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
         <v>147</v>
       </c>
@@ -6316,7 +6344,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B20" s="7" t="s">
         <v>149</v>
       </c>
@@ -6351,7 +6379,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B21" s="7" t="s">
         <v>151</v>
       </c>
@@ -6386,7 +6414,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B22" s="7" t="s">
         <v>153</v>
       </c>
@@ -6421,7 +6449,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B23" s="7" t="s">
         <v>155</v>
       </c>
@@ -6456,7 +6484,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B24" s="4" t="s">
         <v>239</v>
       </c>
@@ -6491,7 +6519,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B25" s="4" t="s">
         <v>240</v>
       </c>
@@ -6526,7 +6554,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B26" s="4" t="s">
         <v>240</v>
       </c>
@@ -6561,7 +6589,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B27" s="4" t="s">
         <v>240</v>
       </c>
@@ -6594,6 +6622,41 @@
       </c>
       <c r="L27" s="4" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B28" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -6610,12 +6673,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1">
+    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6632,7 +6695,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -6663,9 +6726,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6679,7 +6742,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6690,7 +6753,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6701,7 +6764,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4">
         <v>2</v>
       </c>
@@ -6712,7 +6775,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>0</v>
       </c>
@@ -6723,7 +6786,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6734,7 +6797,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7">
         <v>2</v>
       </c>
@@ -6759,16 +6822,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6788,7 +6851,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -6808,7 +6871,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>129</v>
       </c>
@@ -6828,7 +6891,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>131</v>
       </c>
@@ -6848,7 +6911,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>239</v>
       </c>
@@ -6868,7 +6931,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>239</v>
       </c>
@@ -6888,7 +6951,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>239</v>
       </c>
@@ -6922,13 +6985,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -6942,7 +7005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>170</v>
       </c>
@@ -6956,7 +7019,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>171</v>
       </c>
@@ -6970,7 +7033,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>172</v>
       </c>
@@ -6984,7 +7047,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>173</v>
       </c>
@@ -6998,7 +7061,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>174</v>
       </c>
@@ -7012,7 +7075,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>175</v>
       </c>
@@ -7026,7 +7089,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>308</v>
       </c>
@@ -7055,18 +7118,18 @@
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="4"/>
+    <col min="1" max="4" width="8.875" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="4"/>
-    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.875" style="4"/>
+    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>182</v>
       </c>
@@ -7101,7 +7164,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7133,7 +7196,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7173,23 +7236,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.375" customWidth="1"/>
+    <col min="10" max="10" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.83203125" style="4"/>
+    <col min="14" max="15" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7247,8 +7310,11 @@
       <c r="S1" s="10" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="10" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7292,7 +7358,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7339,7 +7405,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7383,7 +7449,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7427,7 +7493,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7474,7 +7540,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7500,7 +7566,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>268</v>
+        <v>73</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -7519,6 +7585,59 @@
       </c>
       <c r="S7" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="T8" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -7535,15 +7654,15 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7569,7 +7688,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7592,7 +7711,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7629,12 +7748,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7657,7 +7776,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7694,12 +7813,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="16384" width="8.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1">
+    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -7710,7 +7829,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B2" s="4" t="s">
         <v>125</v>
       </c>
@@ -7721,7 +7840,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
         <v>125</v>
       </c>
@@ -7732,7 +7851,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
         <v>143</v>
       </c>
@@ -7743,7 +7862,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
#42 change template.xlsx for program relative
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archive\Personal\code\SE\backend\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AC7BAD-95CC-49A4-8A9D-6F8FBEEEC72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908DB933-D990-48F2-8604-F2428EB550E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="38040" tabRatio="832" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="321">
   <si>
     <t>username</t>
   </si>
@@ -1120,6 +1120,22 @@
   </si>
   <si>
     <t>.\files\task\admin_c_1651829254.4129157\6磁场-21_admin_tsk_1651244631_admin_tsk_1651829254.4139159.pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新人培训2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1537,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView topLeftCell="G31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S48" sqref="S48"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5322,8 +5338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5366,8 +5382,8 @@
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
+      <c r="C2" s="4" t="s">
+        <v>210</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -5395,8 +5411,8 @@
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
+      <c r="C3" s="4" t="s">
+        <v>212</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -5421,8 +5437,8 @@
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
+      <c r="C4" s="4" t="s">
+        <v>320</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -5447,8 +5463,8 @@
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
+      <c r="C5" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -5473,8 +5489,8 @@
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
+      <c r="C6" s="4" t="s">
+        <v>314</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -5499,8 +5515,8 @@
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="4">
-        <v>2</v>
+      <c r="C7" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>76</v>
@@ -5525,8 +5541,8 @@
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="4">
-        <v>2</v>
+      <c r="C8" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -5551,8 +5567,8 @@
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="4">
-        <v>2</v>
+      <c r="C9" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -5577,8 +5593,8 @@
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="4">
-        <v>2</v>
+      <c r="C10" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
@@ -5603,8 +5619,8 @@
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="4">
-        <v>2</v>
+      <c r="C11" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
@@ -5629,8 +5645,8 @@
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="4">
-        <v>2</v>
+      <c r="C12" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
@@ -7112,10 +7128,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="194" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView zoomScale="194" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7193,7 +7209,7 @@
         <v>296</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
@@ -7228,9 +7244,394 @@
         <v>125</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="4">
+        <v>4000</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7238,7 +7639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add unitest for get cur role and finish lesson api, add tests in honor api
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LearningResources\CodeAssignment\2022Spring\SoftwareEngineering\backend\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908DB933-D990-48F2-8604-F2428EB550E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A5393A-7B84-7242-9DEF-6AD4E7CD3BF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="38040" tabRatio="832" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="832" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="349">
   <si>
     <t>username</t>
   </si>
@@ -1137,13 +1137,108 @@
   <si>
     <t>5</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:05</t>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:06</t>
+  </si>
+  <si>
+    <t>用于</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finish lesson 测试</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:08</t>
+  </si>
+  <si>
+    <t>用于finish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomer的新人培训</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag2</t>
+  </si>
+  <si>
+    <t>400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lesson测试的course</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomer的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:02</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:03</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:04</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:05</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:06</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:07</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:09</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:10</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:11</t>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:12</t>
+  </si>
+  <si>
+    <t>22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:06</t>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1553,39 +1648,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="4" customWidth="1"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.875" style="4"/>
+    <col min="9" max="9" width="8.83203125" style="4"/>
     <col min="10" max="10" width="11" style="4" customWidth="1"/>
     <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.875" style="4" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="4" customWidth="1"/>
-    <col min="14" max="17" width="8.875" style="4"/>
-    <col min="18" max="18" width="20.625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="21.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="22.625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="16.375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="21.625" style="4" customWidth="1"/>
-    <col min="23" max="23" width="22.875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="23.375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="21.125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="17.875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="18.625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="20.875" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="8.875" style="4"/>
+    <col min="12" max="12" width="21.83203125" style="4" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="4" customWidth="1"/>
+    <col min="14" max="17" width="8.83203125" style="4"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="22.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="16.33203125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="22.83203125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="21.1640625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -1754,7 +1849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28">
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
@@ -1837,7 +1932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>110</v>
       </c>
@@ -1920,7 +2015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>111</v>
       </c>
@@ -2003,7 +2098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
         <v>112</v>
       </c>
@@ -2086,7 +2181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
@@ -2169,7 +2264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
         <v>114</v>
       </c>
@@ -2252,7 +2347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
         <v>115</v>
       </c>
@@ -2335,7 +2430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
         <v>116</v>
       </c>
@@ -2418,7 +2513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
         <v>117</v>
       </c>
@@ -2501,7 +2596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28">
       <c r="A12" s="4" t="s">
         <v>118</v>
       </c>
@@ -2584,7 +2679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28">
       <c r="A13" s="4" t="s">
         <v>119</v>
       </c>
@@ -2667,7 +2762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28">
       <c r="A14" s="4" t="s">
         <v>120</v>
       </c>
@@ -2750,7 +2845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28">
       <c r="A15" s="4" t="s">
         <v>121</v>
       </c>
@@ -2833,7 +2928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28">
       <c r="A16" s="4" t="s">
         <v>122</v>
       </c>
@@ -2916,7 +3011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -2999,7 +3094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28">
       <c r="A18" s="4" t="s">
         <v>128</v>
       </c>
@@ -3082,7 +3177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28">
       <c r="A19" s="4" t="s">
         <v>130</v>
       </c>
@@ -3165,7 +3260,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28">
       <c r="A20" s="4" t="s">
         <v>132</v>
       </c>
@@ -3248,7 +3343,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28">
       <c r="A21" s="4" t="s">
         <v>134</v>
       </c>
@@ -3331,7 +3426,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28">
       <c r="A22" s="4" t="s">
         <v>136</v>
       </c>
@@ -3414,7 +3509,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28">
       <c r="A23" s="4" t="s">
         <v>146</v>
       </c>
@@ -3497,7 +3592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28">
       <c r="A24" s="4" t="s">
         <v>148</v>
       </c>
@@ -3580,7 +3675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28">
       <c r="A25" s="4" t="s">
         <v>150</v>
       </c>
@@ -3663,7 +3758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28">
       <c r="A26" s="4" t="s">
         <v>152</v>
       </c>
@@ -3746,7 +3841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28">
       <c r="A27" s="4" t="s">
         <v>154</v>
       </c>
@@ -3829,7 +3924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28">
       <c r="A28" s="4" t="s">
         <v>156</v>
       </c>
@@ -3912,7 +4007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28">
       <c r="A29" s="4" t="s">
         <v>195</v>
       </c>
@@ -3995,7 +4090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28">
       <c r="A30" s="4" t="s">
         <v>196</v>
       </c>
@@ -4078,7 +4173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28">
       <c r="A31" s="4" t="s">
         <v>197</v>
       </c>
@@ -4161,7 +4256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28">
       <c r="A32" s="4" t="s">
         <v>198</v>
       </c>
@@ -4244,7 +4339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28">
       <c r="A33" s="4" t="s">
         <v>199</v>
       </c>
@@ -4327,7 +4422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28">
       <c r="A34" s="4" t="s">
         <v>200</v>
       </c>
@@ -4410,7 +4505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28">
       <c r="A35" s="4" t="s">
         <v>201</v>
       </c>
@@ -4493,7 +4588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28">
       <c r="A36" s="4" t="s">
         <v>202</v>
       </c>
@@ -4576,7 +4671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28">
       <c r="A37" s="4" t="s">
         <v>203</v>
       </c>
@@ -4659,7 +4754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28">
       <c r="A38" s="4" t="s">
         <v>204</v>
       </c>
@@ -4742,7 +4837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28">
       <c r="A39" s="4" t="s">
         <v>205</v>
       </c>
@@ -4825,7 +4920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28">
       <c r="A40" s="4" t="s">
         <v>206</v>
       </c>
@@ -4908,7 +5003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4982,7 +5077,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28">
       <c r="A42" s="4" t="s">
         <v>238</v>
       </c>
@@ -5056,7 +5151,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28">
       <c r="A43" s="4" t="s">
         <v>239</v>
       </c>
@@ -5130,7 +5225,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28">
       <c r="A44" s="4" t="s">
         <v>240</v>
       </c>
@@ -5204,7 +5299,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28">
       <c r="A45" s="4" t="s">
         <v>257</v>
       </c>
@@ -5336,20 +5431,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C12"/>
+    <sheetView zoomScale="174" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="21.375" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="21.33203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5378,7 +5473,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5407,7 +5502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5420,6 +5515,9 @@
       <c r="E3" s="4">
         <v>1</v>
       </c>
+      <c r="F3" s="4" t="s">
+        <v>335</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>252</v>
       </c>
@@ -5433,7 +5531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5446,6 +5544,9 @@
       <c r="E4" s="4">
         <v>1</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>336</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>259</v>
       </c>
@@ -5459,7 +5560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5472,6 +5573,9 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
+      <c r="F5" s="4" t="s">
+        <v>337</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>251</v>
       </c>
@@ -5485,7 +5589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5498,6 +5602,9 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
+      <c r="F6" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="G6" s="4" t="s">
         <v>252</v>
       </c>
@@ -5511,7 +5618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5524,6 +5631,9 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
+      <c r="F7" s="4" t="s">
+        <v>339</v>
+      </c>
       <c r="G7" s="4" t="s">
         <v>253</v>
       </c>
@@ -5537,7 +5647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5550,6 +5660,9 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>340</v>
+      </c>
       <c r="G8" s="4" t="s">
         <v>254</v>
       </c>
@@ -5563,7 +5676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -5576,6 +5689,9 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
+      <c r="F9" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="G9" s="4" t="s">
         <v>253</v>
       </c>
@@ -5589,7 +5705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -5602,6 +5718,9 @@
       <c r="E10" s="4">
         <v>1</v>
       </c>
+      <c r="F10" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="G10" s="4" t="s">
         <v>250</v>
       </c>
@@ -5615,7 +5734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -5628,6 +5747,9 @@
       <c r="E11" s="4">
         <v>1</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>342</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>254</v>
       </c>
@@ -5641,7 +5763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -5654,6 +5776,9 @@
       <c r="E12" s="4">
         <v>1</v>
       </c>
+      <c r="F12" s="4" t="s">
+        <v>343</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>253</v>
       </c>
@@ -5665,6 +5790,35 @@
       </c>
       <c r="J12" s="4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5675,27 +5829,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:L29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.875" style="4"/>
-    <col min="4" max="4" width="7.875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="4"/>
-    <col min="7" max="7" width="11.375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
-    <col min="9" max="9" width="17.625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="8.875" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
+    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -5730,7 +5884,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -5765,7 +5919,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:12">
       <c r="B3" s="4" t="s">
         <v>130</v>
       </c>
@@ -5800,7 +5954,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>132</v>
       </c>
@@ -5835,7 +5989,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>134</v>
       </c>
@@ -5870,7 +6024,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>136</v>
       </c>
@@ -5905,7 +6059,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>146</v>
       </c>
@@ -5940,7 +6094,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>148</v>
       </c>
@@ -5975,7 +6129,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>150</v>
       </c>
@@ -6010,7 +6164,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:12">
       <c r="B10" s="4" t="s">
         <v>152</v>
       </c>
@@ -6045,7 +6199,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12">
       <c r="B11" s="4" t="s">
         <v>154</v>
       </c>
@@ -6080,7 +6234,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12">
       <c r="B12" s="4" t="s">
         <v>156</v>
       </c>
@@ -6115,7 +6269,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12">
       <c r="B13" s="7" t="s">
         <v>127</v>
       </c>
@@ -6150,7 +6304,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12">
       <c r="B14" s="7" t="s">
         <v>129</v>
       </c>
@@ -6185,7 +6339,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12">
       <c r="B15" s="7" t="s">
         <v>131</v>
       </c>
@@ -6220,7 +6374,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12">
       <c r="B16" s="7" t="s">
         <v>133</v>
       </c>
@@ -6255,7 +6409,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:12">
       <c r="B17" s="7" t="s">
         <v>135</v>
       </c>
@@ -6290,7 +6444,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:12">
       <c r="B18" s="7" t="s">
         <v>145</v>
       </c>
@@ -6325,7 +6479,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:12">
       <c r="B19" s="7" t="s">
         <v>147</v>
       </c>
@@ -6360,7 +6514,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12">
       <c r="B20" s="7" t="s">
         <v>149</v>
       </c>
@@ -6395,7 +6549,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:12">
       <c r="B21" s="7" t="s">
         <v>151</v>
       </c>
@@ -6430,7 +6584,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:12">
       <c r="B22" s="7" t="s">
         <v>153</v>
       </c>
@@ -6465,7 +6619,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12">
       <c r="B23" s="7" t="s">
         <v>155</v>
       </c>
@@ -6500,7 +6654,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:12">
       <c r="B24" s="4" t="s">
         <v>239</v>
       </c>
@@ -6535,7 +6689,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:12">
       <c r="B25" s="4" t="s">
         <v>240</v>
       </c>
@@ -6570,7 +6724,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:12">
       <c r="B26" s="4" t="s">
         <v>240</v>
       </c>
@@ -6605,7 +6759,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:12">
       <c r="B27" s="4" t="s">
         <v>240</v>
       </c>
@@ -6640,7 +6794,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:12">
       <c r="B28" s="4" t="s">
         <v>240</v>
       </c>
@@ -6673,6 +6827,41 @@
       </c>
       <c r="L28" s="4" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -6683,18 +6872,18 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="B1:F2"/>
+  <dimension ref="B1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="302" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="302" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -6711,7 +6900,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>128</v>
       </c>
@@ -6726,6 +6915,40 @@
       </c>
       <c r="F2" s="4" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -6742,9 +6965,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>27</v>
       </c>
@@ -6758,7 +6981,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6769,7 +6992,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3">
         <v>1</v>
       </c>
@@ -6780,7 +7003,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4">
         <v>2</v>
       </c>
@@ -6791,7 +7014,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5">
         <v>0</v>
       </c>
@@ -6802,7 +7025,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6">
         <v>1</v>
       </c>
@@ -6813,7 +7036,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7">
         <v>2</v>
       </c>
@@ -6838,16 +7061,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="20.125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -6867,7 +7090,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -6887,7 +7110,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7">
       <c r="B3" t="s">
         <v>129</v>
       </c>
@@ -6907,7 +7130,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>131</v>
       </c>
@@ -6927,7 +7150,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>239</v>
       </c>
@@ -6947,7 +7170,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7">
       <c r="B6" t="s">
         <v>239</v>
       </c>
@@ -6967,7 +7190,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:7">
       <c r="B7" t="s">
         <v>239</v>
       </c>
@@ -6998,16 +7221,16 @@
   <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView zoomScale="262" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
@@ -7021,7 +7244,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>170</v>
       </c>
@@ -7035,7 +7258,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>171</v>
       </c>
@@ -7049,7 +7272,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>172</v>
       </c>
@@ -7063,7 +7286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>173</v>
       </c>
@@ -7077,7 +7300,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>174</v>
       </c>
@@ -7091,7 +7314,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>175</v>
       </c>
@@ -7105,7 +7328,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>308</v>
       </c>
@@ -7128,24 +7351,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScale="194" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A15"/>
+    <sheetView topLeftCell="E1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="4" width="8.875" style="4"/>
+    <col min="1" max="1" width="8.83203125" style="4"/>
+    <col min="2" max="2" width="20.33203125" style="4" customWidth="1"/>
+    <col min="3" max="4" width="8.83203125" style="4"/>
     <col min="5" max="5" width="12" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="20.625" style="4" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="4"/>
-    <col min="10" max="10" width="18.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.875" style="4"/>
+    <col min="6" max="6" width="18.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="10" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>182</v>
       </c>
@@ -7180,7 +7405,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7212,7 +7437,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7244,7 +7469,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>210</v>
       </c>
@@ -7276,7 +7501,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>211</v>
       </c>
@@ -7308,7 +7533,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>219</v>
       </c>
@@ -7340,7 +7565,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>220</v>
       </c>
@@ -7372,7 +7597,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>221</v>
       </c>
@@ -7404,7 +7629,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>319</v>
       </c>
@@ -7436,7 +7661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
         <v>223</v>
       </c>
@@ -7468,7 +7693,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>224</v>
       </c>
@@ -7500,7 +7725,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>225</v>
       </c>
@@ -7532,7 +7757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
         <v>226</v>
       </c>
@@ -7564,7 +7789,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
         <v>227</v>
       </c>
@@ -7596,7 +7821,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
         <v>228</v>
       </c>
@@ -7625,6 +7850,38 @@
         <v>292</v>
       </c>
       <c r="K15" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7637,23 +7894,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="J1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="4" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="15" width="8.875" style="4"/>
+    <col min="14" max="15" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -7715,7 +7974,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7759,7 +8018,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7806,7 +8065,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7850,7 +8109,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7894,7 +8153,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7941,7 +8200,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7988,7 +8247,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>7</v>
       </c>
@@ -8039,6 +8298,53 @@
       </c>
       <c r="T8" t="s">
         <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -8049,21 +8355,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="20.875" customWidth="1"/>
-    <col min="8" max="8" width="8.875" style="4"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -8089,7 +8395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8112,7 +8418,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8133,6 +8439,29 @@
       </c>
       <c r="H3" s="4" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -8145,16 +8474,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="304" workbookViewId="0">
+    <sheetView zoomScale="304" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="6" max="6" width="8.875" style="4"/>
+    <col min="6" max="6" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -8177,7 +8506,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8208,18 +8537,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="250" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="B1" zoomScale="250" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.875" style="4"/>
+    <col min="1" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1">
       <c r="B1" s="3" t="s">
         <v>57</v>
       </c>
@@ -8230,7 +8559,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4">
       <c r="B2" s="4" t="s">
         <v>125</v>
       </c>
@@ -8241,7 +8570,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:4">
       <c r="B3" s="4" t="s">
         <v>125</v>
       </c>
@@ -8252,7 +8581,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4">
       <c r="B4" s="4" t="s">
         <v>143</v>
       </c>
@@ -8263,7 +8592,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4">
       <c r="B5" s="4" t="s">
         <v>143</v>
       </c>
@@ -8272,6 +8601,17 @@
       </c>
       <c r="D5" s="4" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#50 now finish lesson and finish all lesson unittest teacher newcomer list by name  added
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBB45C1-B7BA-7C40-B44E-38742E475B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DB8776-395A-B449-95D0-3871D4E38460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="41940" windowHeight="18060" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="privateinfo" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="366">
   <si>
     <t>username</t>
   </si>
@@ -1157,10 +1157,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>newcomer的新人培训</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用于测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1180,10 +1176,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>newcomer的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2022-5-3 00:00:02</t>
   </si>
   <si>
@@ -1226,6 +1218,85 @@
   </si>
   <si>
     <t>2022-5-7 00:00:07</t>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:05</t>
+  </si>
+  <si>
+    <t>finishnewcomer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacherCommitted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomerCommitted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>newcomerfinish的新人培训</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finishnewcomer的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finishteacher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导师毕业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学生毕业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-1 23:59:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teacherfinish的导师培训</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-2 00:00:09</t>
+  </si>
+  <si>
+    <t>finish lesson 测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finishteacher的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022-5-3 00:00:13</t>
+  </si>
+  <si>
+    <t>2022-5-6 00:00:07</t>
+  </si>
+  <si>
+    <t>2022-5-7 00:00:08</t>
   </si>
 </sst>
 </file>
@@ -1640,15 +1711,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB45"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="R27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="17.1640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="4"/>
     <col min="4" max="4" width="7.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="16" style="4" customWidth="1"/>
@@ -5260,7 +5332,7 @@
         <v>125</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>248</v>
+        <v>355</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>76</v>
@@ -5337,7 +5409,7 @@
         <v>125</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>247</v>
+        <v>355</v>
       </c>
       <c r="S45" s="4" t="s">
         <v>76</v>
@@ -5352,7 +5424,7 @@
         <v>76</v>
       </c>
       <c r="W45" s="4" t="s">
-        <v>247</v>
+        <v>355</v>
       </c>
       <c r="X45" s="4" t="s">
         <v>76</v>
@@ -5368,6 +5440,160 @@
       </c>
       <c r="AB45" s="4" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
+      <c r="A46" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="R46" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="S46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="T46" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="U46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y46" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB46" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
+      <c r="A47" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="R47" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="S47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="T47" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="X47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y47" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -5417,18 +5643,20 @@
     <hyperlink ref="B40" r:id="rId42" xr:uid="{9BE6E5DB-9ED5-D445-A82F-149B56DE779C}"/>
     <hyperlink ref="B44" r:id="rId43" xr:uid="{3DA1C4FE-DC71-3647-B52C-E065CA59C3B0}"/>
     <hyperlink ref="B45" r:id="rId44" xr:uid="{21C402C8-23D4-EA4C-B714-A7D2D4F747F0}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{6CB51E85-EA28-0E4E-B9CA-026F4DF7D74F}"/>
+    <hyperlink ref="B47" r:id="rId46" xr:uid="{A95C1F43-CBF2-884E-BFE0-468A9B66CD83}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="B1:J13"/>
+  <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -5510,7 +5738,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>252</v>
@@ -5539,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>259</v>
@@ -5568,7 +5796,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>251</v>
@@ -5597,7 +5825,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>252</v>
@@ -5626,7 +5854,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>253</v>
@@ -5655,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>254</v>
@@ -5713,7 +5941,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>250</v>
@@ -5742,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>254</v>
@@ -5771,7 +5999,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>253</v>
@@ -5788,7 +6016,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="4" t="s">
-        <v>240</v>
+        <v>346</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>325</v>
@@ -5800,7 +6028,7 @@
         <v>76</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>253</v>
@@ -5813,6 +6041,35 @@
       </c>
       <c r="J13" s="4" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5823,19 +6080,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:L29"/>
+  <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="8.83203125" style="4"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="4"/>
     <col min="4" max="4" width="7.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4"/>
-    <col min="7" max="7" width="11.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" style="4"/>
     <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" style="4" customWidth="1"/>
@@ -6825,7 +7084,7 @@
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="4" t="s">
-        <v>240</v>
+        <v>346</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>319</v>
@@ -6852,10 +7111,45 @@
         <v>76</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -6866,15 +7160,17 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="B1:F3"/>
+  <dimension ref="B1:F4"/>
   <sheetViews>
     <sheetView zoomScale="302" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="8.83203125" style="4"/>
+    <col min="2" max="2" width="18.1640625" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" s="6" customFormat="1">
@@ -6913,7 +7209,7 @@
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
-        <v>240</v>
+        <v>346</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>210</v>
@@ -6922,10 +7218,27 @@
         <v>76</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -6938,7 +7251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+    <sheetView zoomScale="189" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -7032,10 +7345,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:G7"/>
+  <dimension ref="B1:I8"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7045,9 +7358,11 @@
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1">
+    <row r="1" spans="2:9" s="1" customFormat="1">
       <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
@@ -7066,8 +7381,14 @@
       <c r="G1" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="2:7">
+      <c r="H1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
         <v>128</v>
       </c>
@@ -7086,8 +7407,14 @@
       <c r="G2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>129</v>
       </c>
@@ -7106,8 +7433,14 @@
       <c r="G3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>131</v>
       </c>
@@ -7126,8 +7459,14 @@
       <c r="G4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>239</v>
       </c>
@@ -7146,8 +7485,14 @@
       <c r="G5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>239</v>
       </c>
@@ -7166,8 +7511,14 @@
       <c r="G6" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>239</v>
       </c>
@@ -7185,6 +7536,38 @@
       </c>
       <c r="G7" t="s">
         <v>306</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
+        <v>346</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7328,10 +7711,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="194" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="194" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7835,22 +8218,22 @@
         <v>325</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>328</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>329</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>76</v>
@@ -7860,6 +8243,38 @@
       </c>
       <c r="K16" s="4" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7871,10 +8286,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T18" sqref="K18:T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8288,7 +8703,7 @@
         <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F9">
         <v>20</v>
@@ -8321,7 +8736,54 @@
         <v>0</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -8332,10 +8794,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8439,6 +8901,29 @@
       </c>
       <c r="H4" s="4" t="s">
         <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>360</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -8514,15 +8999,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="250" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="250" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="3" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="15.5" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" s="6" customFormat="1">
@@ -8588,7 +9075,18 @@
         <v>319</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>332</v>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#49 fix some code style bug
</commit_message>
<xml_diff>
--- a/testcase/template.xlsx
+++ b/testcase/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xxy/xcd/大学课件/本学期/软工/大作业/backend/testcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DB8776-395A-B449-95D0-3871D4E38460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFCA9C9-42C1-214C-BCD2-BC0A9576125A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="41940" windowHeight="18060" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1714,7 +1714,7 @@
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="W45" sqref="W45"/>
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>